<commit_message>
View Only Keyword Window WIP
</commit_message>
<xml_diff>
--- a/PG6020.xlsx
+++ b/PG6020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\246767\OneDrive - Spectrum Brands, Inc\Documents\ReviewCampParser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_F8D630C21198C811B0C00D2B08C520B8310809B1" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{BCA4CC2D-596C-4956-AAA2-A66AE282B981}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="11_F8D630C21198C811B0C00D2B08C520B8310809B1" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{11D8B86A-8363-4194-BE72-86F1220AA67C}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="19020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1332" uniqueCount="714">
   <si>
     <t>Amazon</t>
   </si>
@@ -1103,6 +1103,1065 @@
   </si>
   <si>
     <t>2017-03-18</t>
+  </si>
+  <si>
+    <t>2011-07-04</t>
+  </si>
+  <si>
+    <t>Works for only about 4 seconds</t>
+  </si>
+  <si>
+    <t>The instructions indicate that you should charge the device for at least 12-14 hours before use, and trying to use it without doing that charge makes it clear why those instructions exist: The device will turn on for a second or two, then stop working. That's fine, so you charge it for a day and intend to use it the next day.  The problem is, even if you give it up to 24 hours the longest the device will give you a shave for is about 4 seconds, enough time to remove one sideburn.  Is this product a joke? I plugged it in at around 7:00 AM and attempted to use it at around 7:00 AM the following morning. The device cut one of my sideburns, and just turned off. Thankfully I kept my old trimmer so I could just use that one, but this product really seems like you would buy it to play a cruel joke on someone, to see them come into work with half their mustache trimmed or something like that.  The critical flaw with this product is the grossly underpowered motor, power adapter and/or battery. The motor of the device simply isn't strong enough to fight the resistance created by its own attachments that were designed for it. Only if you remove all attachments and look at the spinning metal knob will you realize that the product actually does try to do something, and does have and keeps a charge, but the motor isn't strong enough to move that knob while inside an attachment to do anything significant. The result is the moment you attempt to use even the default attachment, the knob isn't able to move the blades after around 4 seconds of use, and the device dies, even on a full charge.</t>
+  </si>
+  <si>
+    <t>2011-07-08</t>
+  </si>
+  <si>
+    <t>Barely usable</t>
+  </si>
+  <si>
+    <t>The guard is to large to use in areas like mustache. Jabs your nose before it gets to the hair causing you to try to trim your mustache sideways! Lots of settings but lock is not secure. While pressing against face it will move to another setting unless you hold it which is not easy. There is also a lot of flexing of the guard causing different lengths in areas like the chin. The attachments for nose/ear work well as do the other attachments. Overall I find it hard to believe this product made it to production. Testing should have failed.</t>
+  </si>
+  <si>
+    <t>2011-08-05</t>
+  </si>
+  <si>
+    <t>Meh</t>
+  </si>
+  <si>
+    <t>I bought this from a local grocery store as a replacement for multiple tools I used to use that have either stopped working completely, or stopped functioning correctly.  The clippers: This is the main reason I purchased this, and while the clippers without the guard work well, the guard has absolutely no merit on the product itself 'cause it just doesnt work. I cut my own hair, figured this would work and it did but there is no guide as to what length each setting means other than 1,2,3,4,5,etc..  The nose trimmer: For me, this doesn't work at all its nearly too large to actually fit inside my nose and the angles I have to put it at are just obsurd.  The Shaver: This is one of the main reasons I purchased this product as my old remmington shaver stopped working the way it should after a good 10+ years. It worked well for some of my hair, but the closeness of the shave is nowhere near that of a blade razor or my old remmington electric shaver that I had prior to this. I've had the product not very long and now the shaver doesn't work at all. I tried following the industructions to clean it and it just doesn't work.  Product as a whole: I brought the product home, unpackaged it and read the instructions before doing anything with it. It said to charge it for a while before use so I plugged it in. Problem is the plug wouldn't stay inside the shaver unit itself long enough to charge the batteries or so I thought.  I cracked open the unit (no screws hold it together), and noticed that the ground wire on the charging circut board the entire solder joint had broken apart. So if the solder point wasnt touching the circut board, it wasnt charging (no light).. I fixed this myself bu melting the solder, and adding a little bit more. It now charges, but not every consumer is going to own or know how to solder something together.  The motor when no attachments are on it seems very strong, but once you add an attachment it seems to get very weak which could result in hair being pulled out instead of cut.  I've only owned this unit for about 7 days now and I've already gone through these issues with the product. There are only a few ways i'd recommend this product and these are as follows:  1. you know how to solder (by the other reviews about no charging taking place, seems like you'll have to). 2. you throw away the guides, the nose trimmer, the foil shaver, and everything else but the clipper portion. 3. you intend to use it for nothing more than shaving your long haired animals.  If all 3 of the above are true, then by all means spend the money but otherwise do yourself a favor and buy a better product if you have the money.</t>
+  </si>
+  <si>
+    <t>2011-09-13</t>
+  </si>
+  <si>
+    <t>Great tool for me</t>
+  </si>
+  <si>
+    <t>I went in looking for 2 products. One for nose and one to trim off my beard so I could shave. I found this one for a little more than a nose hair trimmer costs, and it seemed to say it did so much more. I've used the hair and beard trimmer guides, the shaver, nose hair cutter. The only adapter I haven't used is the rocking detailer thing. All the parts have worked great for me. I'm working up the nerve to try the hair trimmer for an at home haircut. The number guides on the guards make great sense to me and work well.</t>
+  </si>
+  <si>
+    <t>2011-10-10</t>
+  </si>
+  <si>
+    <t>it does what it says it does</t>
+  </si>
+  <si>
+    <t>ok for the price it does what it needs to do i got it to trim around my beard and it did a great job. if u need a small light wight trimmer i think it does the job it not a full time shaver so i did not expect it to do that. so for the money it was worth it</t>
+  </si>
+  <si>
+    <t>2011-10-15</t>
+  </si>
+  <si>
+    <t>Worst bang for your buck</t>
+  </si>
+  <si>
+    <t>I purchased this product as a temp trimmer. Worst idea ever. It pulls not cuts. Very painful experience</t>
+  </si>
+  <si>
+    <t>2011-11-14</t>
+  </si>
+  <si>
+    <t>Great Product</t>
+  </si>
+  <si>
+    <t>I have always been satisfied with Remington's products. However, this one is my favorite! It's great for on the go touch up's and for all body parts! Thanks Remington!</t>
+  </si>
+  <si>
+    <t>2011-11-28</t>
+  </si>
+  <si>
+    <t>Works perfect</t>
+  </si>
+  <si>
+    <t>I love that this trimmer is cordless and you don't need to oil it after use. Those two things alone make this product perfect.</t>
+  </si>
+  <si>
+    <t>2011-11-30</t>
+  </si>
+  <si>
+    <t>Gets the job done!</t>
+  </si>
+  <si>
+    <t>This product really takes care of everything, whether I'm going for the last minute buzz cut or just touching up this chargeable trimmer is very user friendly. I love the quickly swappable pieces and carrying case.  I wish there was a spot for the charging cord in the case.  Excellent value.</t>
+  </si>
+  <si>
+    <t>2011-12-04</t>
+  </si>
+  <si>
+    <t>Great value</t>
+  </si>
+  <si>
+    <t>This product is well worth the money. Compared to other shavers i've had in the past this one is much more convenient. The multiple changeable heads and case is nice.  The only downside i've seen is that some of the heads don't turn into place. This had no effect on the functionality however.</t>
+  </si>
+  <si>
+    <t>2011-12-06</t>
+  </si>
+  <si>
+    <t>Solid</t>
+  </si>
+  <si>
+    <t>I received this all in one system on Wednesday and was finally able to use it over the weekend. I have used a number of other trimmers/groomers in the past so that gives me a good basis for comparison here.  First off, I was glad to see that my device was shipped to me charged. This is a benefit for anyone who doesn't want to waste time charging the product for 12 hours before they can use the item they just purchased. I don't know if they all ship charged or I just got lucky, but that was a plus in my book.  The carrying case included that contains all the variety of heads and bells &amp; whistles was a great touch, although I'm not sure how often I will bring this product on trips due to the nature of its use cases.  The product itself performs admirably in its core roles, and is definitely precise enough for more intimate operations.  I haven't run a full charge down yet, so I can't comment on battery life or durability specifically, but it appears to have a strong battery shelf life and to be fairly robust as a whole.  If I was in the market again I would lean towards purchasing this set.</t>
+  </si>
+  <si>
+    <t>2011-12-13</t>
+  </si>
+  <si>
+    <t>All In One Grooming System</t>
+  </si>
+  <si>
+    <t>Overall this product worked well aside from the Foil Shaver Attachment which didn't really work well at all. It could be made a bit more durable as the plasticness felt like it wasn't going to hold up. Overall the other attachments worked great and I would recommend this based on that and the value of it.</t>
+  </si>
+  <si>
+    <t>2012-01-23</t>
+  </si>
+  <si>
+    <t>Cant hold a charge</t>
+  </si>
+  <si>
+    <t>Don't buy this product. It cannot hold a charge longer than 2 minutes and takes FOREVER to recharge to only 'perform' for like 2 minutes.</t>
+  </si>
+  <si>
+    <t>2012-02-06</t>
+  </si>
+  <si>
+    <t>Product will not hold a complete charge</t>
+  </si>
+  <si>
+    <t>Received this product as a gift. Charged it according to the instruction manual. When turned on, it performed as if it needed charged. I discharged the unit completely, then charged it again per the instruction manual and still it does not perform as if it is charged.  This is the only Remington product that I have been dissatisfied with in the past 25 years of using Remington products.</t>
+  </si>
+  <si>
+    <t>2012-02-14</t>
+  </si>
+  <si>
+    <t>Terrible and Dissappointed</t>
+  </si>
+  <si>
+    <t>This product is a piece of garbage. I was only able to use it once, and now it won't hold a charge. DON'T waste your money on this!</t>
+  </si>
+  <si>
+    <t>2012-02-27</t>
+  </si>
+  <si>
+    <t>Do not buy.</t>
+  </si>
+  <si>
+    <t>This product is horrible in every sense of the word. I have had the device for 2 weeks and it is already worthless. It will not charge, and if it does charge the device will only perform for a maximum of 30 seconds. It is absolutely ridiculous how bad the product performs. I cannot imagine any of these cheap personal groomers are going to be any better. You are honestly better off taking the cash it takes to buy this product and trying to shave with that.</t>
+  </si>
+  <si>
+    <t>2012-03-04</t>
+  </si>
+  <si>
+    <t>BETTER INSTRUCTIONS NEEDED</t>
+  </si>
+  <si>
+    <t>Have used it for 2 weeks--first complaint is that pieces do not fit into 'case' securely--case itself is very flimsy--not all pieces fit in proper allotted spaces. I have not had problems as others seem to have with charging and length of times in between charging. I have tried all the pieces and have not had luck with hair clipper and beard clipper--I may be using them wrong but have no way to tell as instructions don't help. I will use it as a nose, eyebrow and ear trimmer, possibly for mustache trimmer but as far as beard and hair I either will have to experiment more or just use a good old soap, water and razor</t>
+  </si>
+  <si>
+    <t>2012-05-21</t>
+  </si>
+  <si>
+    <t>Lacks Reliabilty</t>
+  </si>
+  <si>
+    <t>When working it does fine... However, it will NOT hold a charge, and it takes forever to charge even just for one "limited" use. Thus it seldom ever works well. Too bad probably could be a good product.. Definitely not worth the money</t>
+  </si>
+  <si>
+    <t>2012-06-07</t>
+  </si>
+  <si>
+    <t>Waste of money!!!</t>
+  </si>
+  <si>
+    <t>Was able to get one use out of this...won't hold a charge. Kept plugged in and charging overnight. NOTHING!!! I would not waste your money on this. I am upset I don't have the packaging to return it and get my money back.</t>
+  </si>
+  <si>
+    <t>2012-06-14</t>
+  </si>
+  <si>
+    <t>Waste of money and time</t>
+  </si>
+  <si>
+    <t>Bought this because I have a similar item from another company at home and forgot it on a three week trip. I use them to shave my head and chest and this could not do either. I don't imagine it would work for facial hair either seeing as mine would barely cut any hair. I pushed through and managed to get a very uneven cut on my head. I thought maybe they were having a rough time with my head hair so I tried using it on my chest hair and that was even worse. Had to go buy another set of clippers just to finish the job. Leaves tons of hair behind and will not cut closs to the skin at all. What a waste of money. Horrible product.  On another note it took me nearly 20 minutes to get a somewhat even cut on my head and I never had a problem with the battery. (not that a battery does any good when the clippers don't work)</t>
+  </si>
+  <si>
+    <t>2012-06-23</t>
+  </si>
+  <si>
+    <t>GOOD PRODUCT, MANY FEATURES</t>
+  </si>
+  <si>
+    <t>THE ALL-IN-1 GROOMING SYSTEM DOES WHAT IT IS DESIGNED TO DO. I HAVEN'T HAD IT FOR VERY LONG BUT I AM FAVORABLY IMPRESSED WITH IT. THE ONLY DOWNER IS THAT THERE IS NOT A WAY TO KNOW WHEN THE BATTERY IS FULLY CHARGED. THE LIGHT ON MY REMINGTON SHAVER TURNS RED WHEN IT NEEDS TO BE CHARGED BUT THIS ONE STAYS GREEN ALL THE TIME. SO, I GUESS YOU HAVE TO USE IT UNTIL IT BEGINS TO SLOW DOWN AND THEN HOOK IT UP TO THE CHARGER.?</t>
+  </si>
+  <si>
+    <t>2012-06-24</t>
+  </si>
+  <si>
+    <t>Zero battery life</t>
+  </si>
+  <si>
+    <t>Very disappointed in this product. I bought this to replace an electric razor that I had for years that finally gave out. I have had this Remington for a couple months and the battery life is just awful. I use it to shave my head and trim my goatee. At first the battery held a charge but now it slows down and pretty much dies after about 1 minute of use (even after it charges fully). Would not recommend this item.</t>
+  </si>
+  <si>
+    <t>2012-07-04</t>
+  </si>
+  <si>
+    <t>Great product</t>
+  </si>
+  <si>
+    <t>Fits all my needs. I stay groomed fully from the kneck up.</t>
+  </si>
+  <si>
+    <t>2012-08-25</t>
+  </si>
+  <si>
+    <t>Very dissapointed</t>
+  </si>
+  <si>
+    <t>All around terrible, poor cutting performance ,terrible charging performance,sloppy adjust ability.</t>
+  </si>
+  <si>
+    <t>2012-09-13</t>
+  </si>
+  <si>
+    <t>hairy face</t>
+  </si>
+  <si>
+    <t>poor charging system! Won't hold a charge! Waste of money, very disappointed!</t>
+  </si>
+  <si>
+    <t>2012-09-14</t>
+  </si>
+  <si>
+    <t>What kind of grooming?</t>
+  </si>
+  <si>
+    <t>I have bought quite a few different trimmers, and this one is horrible. This thing doesn't trim neatly infact it trims unevenly. 3 Times I have used it and all 3 times it has destroyed my facial hair style on the same setting it would trim spots shorter then others, no other trimmer has done this to me before, it is also almost impossible to get the hair under your nose on your mustache considering the trimmer attachment is about 1/2 to 1 inch give or take long. As far as the 30 minute run time... I have yet to use it for more then 5 minutes without the battery loosing power and starting to pull hair instead of cut hair. I will be very skeptical on any future remington products I purchase if I ever do, I will be sending this trimmer back to remington telling them to keep the peice of garbage. You have been warned</t>
+  </si>
+  <si>
+    <t>2012-09-24</t>
+  </si>
+  <si>
+    <t>Easy to use</t>
+  </si>
+  <si>
+    <t>This razor is not bad at all. I was worried with all the bad reviews that it would not work at all. However, my husband used the razor to shave his face and his head and the battery was charged the entire time. So no issues with the battery dying. It is very easy to change the razor heads to use either the nose trimmer or the arc detailer. The razor is also very light so easy to hold and handle. For such a great price this razor did everything that he needed to use it for.</t>
+  </si>
+  <si>
+    <t>2012-10-05</t>
+  </si>
+  <si>
+    <t>Not brilliant</t>
+  </si>
+  <si>
+    <t>Got this item for my husband to use and he told me it was a joke of a groomer. He said it worked fine for light trimming but if you want to shave, forget about it. Doesnt get the job done. It didnt keep a good charge at all, very dissapointing for a Remington product. There were a ton of other grooming kits that had much better review so I will try another one.</t>
+  </si>
+  <si>
+    <t>2012-10-19</t>
+  </si>
+  <si>
+    <t>No title</t>
+  </si>
+  <si>
+    <t>Trimmer worked well. However, the hair tends to get stuck in the clippers so you have to manually have to clean it off every so often.</t>
+  </si>
+  <si>
+    <t>2012-10-25</t>
+  </si>
+  <si>
+    <t>Don't Bother</t>
+  </si>
+  <si>
+    <t>Bought this 6 months ago and it's junk. Battery would hold a charge to finish the job and won't run when plugged in. Now 6 months later the battery won't even take a charge. Don't waste your money on this PG</t>
+  </si>
+  <si>
+    <t>Terrible!!!!</t>
+  </si>
+  <si>
+    <t>My wife bought this for me for Chirstmas last year and this thing is terrible. I charge it for an hour and it runs for 1 minutes and stops. It states "no lubrication" and I think that is why it stops working. I pop the top off and turn it on and the internal piece spins but once the attachment is on it stops!!!! TERRIBLE!!!! My old shaver I had for 4 years and had no problems other then the top broke.</t>
+  </si>
+  <si>
+    <t>2012-10-29</t>
+  </si>
+  <si>
+    <t>GReat for in-between haircuts!</t>
+  </si>
+  <si>
+    <t>I typically use this to keep the sideburns and back of my neck tidy in between schedule hair cuts. The clipper holds a charge for quite a while and the different heads make it super easy to switch. It's a great item to have on hand for those last minute touch-ups!</t>
+  </si>
+  <si>
+    <t>2012-11-13</t>
+  </si>
+  <si>
+    <t>Beard became full of holes</t>
+  </si>
+  <si>
+    <t>My beard became full of holes, like failed spots, this happens because of two reasons: the clip is not stable, for example, you set for 4, and suddenly, with any little pression goes to 1, and there's a hole. Another reason is the smallest clip, it has a hop in the middle, and with it, it's easy to cut a little more than you want in the face curved areas.</t>
+  </si>
+  <si>
+    <t>2012-11-16</t>
+  </si>
+  <si>
+    <t>Price is good and it works well</t>
+  </si>
+  <si>
+    <t>2012-11-21</t>
+  </si>
+  <si>
+    <t>REMINGTON PERSONAL GROOMER</t>
+  </si>
+  <si>
+    <t>This groomer works great,its the most versatile groomer I had ever owned and I wont own any other brand.You can't go wrong with a REMINGTON Brand product!!</t>
+  </si>
+  <si>
+    <t>2012-11-30</t>
+  </si>
+  <si>
+    <t>Love the product, hate the battery</t>
+  </si>
+  <si>
+    <t>I really love this product. It has just about everything you need for personal grooming. The blades are sharp and it cuts very well. It does a wonderful job and is a great value to me for the money. The reason I am giving it only 2 stars is because if you do not leave the trimmer on a constant charge you cannot use it. My other trimmer would last sometimes weeks on a full charge. This trimmer will be totally drained the next day. Again, keep in mind what you paid. If you could use the trimmer while plugged would be a great asset. However the poor retention of a full charge is why I give it only 2 stars. I would have gladly spent more for a longer charge. I just do not like leaving things plugged in constantly. Great trimmer, poor battery. Come on, Remington. I would only recommend this product if you don't mind leaving things plugged in all the time.</t>
+  </si>
+  <si>
+    <t>2012-12-20</t>
+  </si>
+  <si>
+    <t>Do Not Buy</t>
+  </si>
+  <si>
+    <t>This was my first electric trimmer and managed to be an extremely disappointing experience. The battery life is only good for maybe 2-3 strokes. I can't even get a part of my neck done with this thing before it cuts out. Leave it plugged in for days and it still doesn't last more than a few seconds. How does trash like this even make it to the market?</t>
+  </si>
+  <si>
+    <t>2012-12-25</t>
+  </si>
+  <si>
+    <t>Bought these for my sons' for Christmas! They Love them! Perfect gifts!</t>
+  </si>
+  <si>
+    <t>2013-01-11</t>
+  </si>
+  <si>
+    <t>I purchased this a few months ago. Worked after the first charge then will not hold charge. Rarely used it and thus did not realize how bad the charge was. Now too late for store return or any warranty. Useless unless used when plugged in.</t>
+  </si>
+  <si>
+    <t>2013-01-28</t>
+  </si>
+  <si>
+    <t>I purchased this a few months ago. While it did the job of what I needed, touching up and maintaining, per say, it didn't take long before it became trash worthy. PROS: One positive thing about this, is the storage case it comes in. Too bad I cannot use it for the one I just purchased. CONS: One of the main heads stopped working. Thought it was something with the actual unit until I tested it to the smaller of the two heads. The foil head is a complete joke. If you want a true electric shaver, buy one. Don't use a head that looks like it could only trim air ... not hair. Second, I noticed that the unit wouldn't maintain a decent charge. It would charge for several hours and then die in less than 5 minutes. Charge it again, would run full steam and just die as if power cord was taken out from outlet. So, no, I would not buy this again, or anything from Remington. In fact, after trying one more time to use the unit, went to WalMart and purchased a Norelco. I've never had an issue with Norelco ... Remington, I've always seem to have some sort of issue to it. So, for about the same amount of money, purchase the Norelco. The only thing negative about the Norelco I purchased, the bag that comes with it to store the unit and attachments, seems nothing more than the bag that comes with the alcoholic bag (initials "C.R."). As mentioned earlier, I at least give credit to the Remington for the case that stores everything, except the plug itself.</t>
+  </si>
+  <si>
+    <t>2013-02-04</t>
+  </si>
+  <si>
+    <t>All in one</t>
+  </si>
+  <si>
+    <t>Reading instructions I can't seem to figure out how to use this thing to trim my mustache . My old trim was great . Put on guide,turn on and trim. It died after years of service and my wife purchased this for me. The guides don't allow trimmer to get anywhere near my mustache. Looked for video on line to see what I was doing wrong, no such luck. Sure hope don't have any problem returning this as I had to rip the box to get at it. Too ad, so sad.</t>
+  </si>
+  <si>
+    <t>2013-02-11</t>
+  </si>
+  <si>
+    <t>A worthless item..tarnises the Remington brand name</t>
+  </si>
+  <si>
+    <t>A piece of junk! Picked this up at Sam's Club several months ago. Battery will not hold a charge. Motor mechanism is not nearly powerful enough to handle facial hair. Don't waste your money!</t>
+  </si>
+  <si>
+    <t>2013-02-22</t>
+  </si>
+  <si>
+    <t>DO NOT BUY!!!!!!!!!!!!!!!</t>
+  </si>
+  <si>
+    <t>I purchased this product thinking that I had a nice new trimmer but little did I know what I was in for.I used it 1 time and I can honestly can say that I was pleased how it worked.The 2nd time I used it I charged it up for about 5 hours and then when I went to use it I cut only a little off my beard and it died,so I finished my beard with a blade.The 3rd and final time I charged it overnight and again when I went to use it it died after doing about half my face so I decided to try finishing my face with the power cord plugged in and that didn't work either,(I guess you cant use it while it is charging like some other things)Then I thought something was wrong with my specific trimmer until I read other user reviews stating the same thing.I took my receipt and trimmer back to Walmart and returned it for a different brand (Wahl) a doubleAA battery trimmer and I couldn't be more happier!</t>
+  </si>
+  <si>
+    <t>2013-02-28</t>
+  </si>
+  <si>
+    <t>I like what it has to offer, but very dissatisfied with the battery life.</t>
+  </si>
+  <si>
+    <t>My wife bought this small convienient razor as a Christmas gift for me. After reading the instructions and charging as it said, i used it and it died within a minute of trimming my face. I thought maybe it would take a few charges to get the battery conditioned. Im wrong so far. I cannot get the battery to hold a charge. For the one minute it does work, it works good. But Im going to contact customer service to see if we can get this corrected.</t>
+  </si>
+  <si>
+    <t>2013-03-23</t>
+  </si>
+  <si>
+    <t>Please don't buy this</t>
+  </si>
+  <si>
+    <t>This product can only be use once and then become trash or recycle material. It won't charge at all. I just wonder Remington will give my money back or do some research before bringing their product into market.</t>
+  </si>
+  <si>
+    <t>2013-03-29</t>
+  </si>
+  <si>
+    <t>dont get it.</t>
+  </si>
+  <si>
+    <t>my sister bought this for me. bab battery life and for some reason the main part that cuts the hair broke..it just dont move.!! propably the worst i ve ever had.</t>
+  </si>
+  <si>
+    <t>2013-04-17</t>
+  </si>
+  <si>
+    <t>Not worth it...</t>
+  </si>
+  <si>
+    <t>Bought this product after using other Remington shavers and am completely disappointed. The battery life is horrible. Lucky if you get a couple minutes of good use and then it dies. Use it for on the go trimming??? Only if you can wait 24 hours for it to have enough juice to actually do something. The shaver attachment is mediocre at best. I was a loyal Remington user, but not any more.</t>
+  </si>
+  <si>
+    <t>2013-06-17</t>
+  </si>
+  <si>
+    <t>Terrible Product!!!</t>
+  </si>
+  <si>
+    <t>I bought it about 2 months ago. It worked great for the first month. Then, the battery would not charge. What a waste of money. I thought Remington was a good product. DO NOT BUY!!! Any product that lasts one month is pathetic. I only actually used it around 6 times to trim my mustache and goatee. No matter how long it stays plugged in, the charge only lasts enough for 15 seconds of use. Go with a brand that works better. I am very disappointed in Remington for selling such poor products.</t>
+  </si>
+  <si>
+    <t>2013-06-23</t>
+  </si>
+  <si>
+    <t>Useless Battery life</t>
+  </si>
+  <si>
+    <t>The product itself is fine. It trims neatly and well, with lots of different attachments. However, it does not hold a charge to save it's life. You are lucky to get a minute or two of shaving out of it after several hours of charging. If you want to do any measurable shave out of it, you need to leave it on the charger overnight, and MAYBE it will last 5 mins.  Do not suggest buying.</t>
+  </si>
+  <si>
+    <t>2013-07-06</t>
+  </si>
+  <si>
+    <t>Upgrade from the PG-250 and PG-350</t>
+  </si>
+  <si>
+    <t>I purchased this unit to replace my old PG-350. The PG6020 is amazing! I just finished my first beard trim with this product and the results are superb. The quality in both the groomer body and the clips is the best I've seen in Remington products at the beard trimmer level. Say good bye to adjustable clips. You get 3 stubble combs that attach to the full-size trimmer that don't adjust. The way the clips themselves attach to the full-size trimmer attachment is another sign of quality, the plastic is hard and durable, and you won't have to worry about the stubble combs breaking. I also used the full-size trimmer to clean up the nape of my neck and my beard line. I can't complain. Then I used the Arc Detailer for my beard line, mustache, and eye brows. The arc detailer trim was very clean and very close to my skin. No remaining stubble. If you are replacing your PG-250 or PG-350 get this item. If you haven't considered replacing your PG-250 and PG-350, I would consider getting the PG6020. [This review was collected as part of a promotion.]</t>
+  </si>
+  <si>
+    <t>2013-08-06</t>
+  </si>
+  <si>
+    <t>Poor Quality</t>
+  </si>
+  <si>
+    <t>I cannot believe, even in this world of disposables that you could manufacture, and market such an inferior quality item. I bought this 2 months ago and it worked good maybe once. Now it will not hold a charge long enough to trim my mustache nor my beard.</t>
+  </si>
+  <si>
+    <t>2013-09-14</t>
+  </si>
+  <si>
+    <t>junk battery life</t>
+  </si>
+  <si>
+    <t>Used one time and worked great, however went to use it today and the battery wont charge, and it will not run on the charging cord!!!!!! [This review was collected as part of a promotion.]</t>
+  </si>
+  <si>
+    <t>2013-09-24</t>
+  </si>
+  <si>
+    <t>Worst Clipper I've Ever Owned</t>
+  </si>
+  <si>
+    <t>This is the worst clipper I've ever owned. After having followed the directions for charging the clipper the first time, I proceeded to cut my hair. It ran out of batteries only a 1/3rd of the way through cutting my hair, leaving me in an awkward position... I had to charge the clipper again for an hour to get 3 to 5 minutes more of weak cutting time.  To make matters worse, the clipper can't run on direct power from the charger. So you can't leave it plugged in and run off of that.  I don't know why Remington is selling this!</t>
+  </si>
+  <si>
+    <t>2013-10-06</t>
+  </si>
+  <si>
+    <t>great price, but does not run while charging.</t>
+  </si>
+  <si>
+    <t>2013-10-27</t>
+  </si>
+  <si>
+    <t>this product has exactly what I need.</t>
+  </si>
+  <si>
+    <t>I am on my second one. I wore the first one out. I like the new designed storage tray better than the older one. They are not expensive so I will buy as many as I can wear out. It is perfect for trimming my mustache and ear and nose hair. Everything is right there. I charge it once a week and it is ready to go.</t>
+  </si>
+  <si>
+    <t>2013-10-31</t>
+  </si>
+  <si>
+    <t>works well</t>
+  </si>
+  <si>
+    <t>Good value!</t>
+  </si>
+  <si>
+    <t>2013-11-03</t>
+  </si>
+  <si>
+    <t>Battery does not last</t>
+  </si>
+  <si>
+    <t>DO NOT PURCHASE THIS PRODUCT.  I purchased a Remington1 all-in-one grooming system about a month ago and it is the worst grooming kit I have ever purchased.  The shaver runs off of battery only, can't be used while plugged into an electrical outlet. The batter barley lasts long enough to shave my head or trim my beard.  I do not recommend this product.</t>
+  </si>
+  <si>
+    <t>2013-11-14</t>
+  </si>
+  <si>
+    <t>Non Existant Battery Life</t>
+  </si>
+  <si>
+    <t>Bought the All in 1 Grooming system and was extremely disappointed with the product. Can bearly manage one beard trimming before the battery is complete dead.</t>
+  </si>
+  <si>
+    <t>2013-11-24</t>
+  </si>
+  <si>
+    <t>My wife bought this for me a few months ago. It worked great for the first month or so and now it doesn't hold a charge. That wouldn't be a big deal if it could be used while plugged in but that doesn't work either. I have left it plugged in for several days at a time, unplugged it and put it away. Then when I take it out to use it, the battery is completely dead. I don't know how this product has not been discontinued after all of the reviews it has gotten about this same problem. Very dissapointed and I won't be buying Remington products anymore.</t>
+  </si>
+  <si>
+    <t>2013-12-02</t>
+  </si>
+  <si>
+    <t>Great cutting but doesn't last long</t>
+  </si>
+  <si>
+    <t>Pros: As a grooming tool I liked all of the attachments and it fits well in your hand. It does a good job at doing what it was made for.  Cons: The stand it comes in does not function well unless your just into displaying your stuff. The cord comes around the front of the stand in order to plug into the shaver as it barely sits in it's cradle.  The battery gave out six months into use. I could live with the rest of the shortcomings of this unit but not this one.  I would not recommend this product.</t>
+  </si>
+  <si>
+    <t>2013-12-04</t>
+  </si>
+  <si>
+    <t>Poor performance</t>
+  </si>
+  <si>
+    <t>I purchased this product to replace an old trimmer made by a competitor that had served me for years. I selected this model because it had a greater variety of attachments than comparable products, and I figured it would be versatile. Given that this is a low-cost product, my expectations were modest, but the product failed to meet even those modest expectations.  As others pointed out, the battery life is the biggest drawback. Even when brand new and fully charged, the battery affords me a scant ten minutes of usage time. Normally, that wouldn't be a problem, since I can trim my beard in ten minutes. However, the blades on the unit are so dull that they continuously jam and clog, even on the thinnest parts of my beard, resulting in painful pulling. I have to make at least six or seven passes over each part of my beard just to get a basic trim.  The result is that I can only ever trim about a third of my beard with this product, then I end up finishing off with scissors and a comb. Overall, this is one of the poorest-performing consumer products I've ever purchased. I strongly advise against purchasing it.</t>
+  </si>
+  <si>
+    <t>2013-12-05</t>
+  </si>
+  <si>
+    <t>Wasted Money</t>
+  </si>
+  <si>
+    <t>As others have said, this product's battery life is completely inadequate. It's still new, and I can't get through a full trim if I've let my beard grow a week or so. I'm satisfied with the trimmer features well enough, considering the money spent. But at any price, this tool just isn't up to the job. I'm sorry I bought it.</t>
+  </si>
+  <si>
+    <t>2013-12-15</t>
+  </si>
+  <si>
+    <t>Convient beard trimmer</t>
+  </si>
+  <si>
+    <t>Trimmer does a lot. A little less powerful for a full beard shave. Excellent for mustaches and goatees, which is why I bought this item anyway.</t>
+  </si>
+  <si>
+    <t>2013-12-25</t>
+  </si>
+  <si>
+    <t>This product is trash.</t>
+  </si>
+  <si>
+    <t>The power delivery system on my clipper fails and the battery life is nonexistent. The clipper will not work without a power cord and even with a power cord it must be charged for about an hour before use. Then, when it does work, the power drains so quickly that it renders the clipper useless.  I had presumed that it was just my clipper that was defective, but I have read countless reviews by others who had the same problem. I did not expect much from this inexpensive product, but I expected more than what it offered me. This product makes a good target for shooting practice.</t>
+  </si>
+  <si>
+    <t>Pay More &amp; Get Less</t>
+  </si>
+  <si>
+    <t>Typical in today's industry you always pay more &amp; get less, the picture isn't what you get. The base or holder doesn't hold anything, the parts just slid. It pulls and doesn't cut well, not sure if it will hold up as to the description.</t>
+  </si>
+  <si>
+    <t>Tried to use it once</t>
+  </si>
+  <si>
+    <t>Immediately threw it in the trash as complete junk.</t>
+  </si>
+  <si>
+    <t>2014-01-09</t>
+  </si>
+  <si>
+    <t>Great Trimmer</t>
+  </si>
+  <si>
+    <t>highly recommend getting this trimmer is worth every penny.</t>
+  </si>
+  <si>
+    <t>2014-01-16</t>
+  </si>
+  <si>
+    <t>Inexpensive &amp; does the job</t>
+  </si>
+  <si>
+    <t>I've had this product for several years and found it to do what its supposed to do, does'nt need oiling, ever, and it can be cleaned with water. Try to remember to charge it up before you use it and it will do what the company says it will.</t>
+  </si>
+  <si>
+    <t>2014-01-18</t>
+  </si>
+  <si>
+    <t>Battery gives me fits</t>
+  </si>
+  <si>
+    <t>My beard isn't exceptionally thick, so I don't require a whole lot. Still, it's frustrating that I need to have the unit already charging for a few hours at the time that I use it. Before that, I'd leave it to charge for most of the day when I go to work, and there is essentially no usable battery life for the next time I trim about a day-and-a-half later.</t>
+  </si>
+  <si>
+    <t>2014-01-23</t>
+  </si>
+  <si>
+    <t>Just what I wanted</t>
+  </si>
+  <si>
+    <t>This is just what I wanted to buy for a few years now.</t>
+  </si>
+  <si>
+    <t>2014-02-19</t>
+  </si>
+  <si>
+    <t>To me this product is fine.</t>
+  </si>
+  <si>
+    <t>I had mines for 2 years and it still works fine i never had a problem with it only thing is you have to clean out the hair and treat it like a lady lol.</t>
+  </si>
+  <si>
+    <t>2014-02-21</t>
+  </si>
+  <si>
+    <t>Product has great versatility.</t>
+  </si>
+  <si>
+    <t>The product consists of enough different attachments to maintain all aspects of beard and mustache trimming. Each attachment is well suited for each different required area to be maintained. Each attachment is easily removed and cleaned and ready for its next use. The main unit is easily charged with its built in charger. The battery, when properly charged, lasts for many uses before required recharging of the battery. I am very pleased with my choice and with the purchase price.</t>
+  </si>
+  <si>
+    <t>2014-02-24</t>
+  </si>
+  <si>
+    <t>Very small teeth make for slow going</t>
+  </si>
+  <si>
+    <t>I bought this to replace a long-serving Norelco that I used for years for general trimming of my full beard - I keep it pretty short. This Remington has much shorter/smaller teeth - it does a decent job but takes 3X as long. I'll stick with it 'cause I'm cheap, but do not recommend it, at least for this purpose.</t>
+  </si>
+  <si>
+    <t>2014-02-25</t>
+  </si>
+  <si>
+    <t>Excellent Product!</t>
+  </si>
+  <si>
+    <t>Had it before and went directly to the remington website to get it again. Great product, what any men should have in their home.</t>
+  </si>
+  <si>
+    <t>2014-02-26</t>
+  </si>
+  <si>
+    <t>Battery life is awful !</t>
+  </si>
+  <si>
+    <t>As I see many people has reported it before me, so I don't want to write about it a lot. Just a quick note, short battery life and to be out of work when the clipper is plugged are two important drawbacks of the product.</t>
+  </si>
+  <si>
+    <t>2014-03-23</t>
+  </si>
+  <si>
+    <t>Don't buy!</t>
+  </si>
+  <si>
+    <t>Battery is terrible. I charge it for hours and it dies very quick. Has to be charged every day. Have had it for a few months and it wont work anymore. Do not spend your money on this.</t>
+  </si>
+  <si>
+    <t>2014-03-26</t>
+  </si>
+  <si>
+    <t>Battery</t>
+  </si>
+  <si>
+    <t>Worst battery life of any groomer I have had. Waste of money.</t>
+  </si>
+  <si>
+    <t>2014-03-27</t>
+  </si>
+  <si>
+    <t>battery died</t>
+  </si>
+  <si>
+    <t>I used this product for 2 years and the battery died - it would run only for 30 sec after charging for 24 hrs. I tried to find a replacement battery but could not. It's kind of sad to throw away a working device because you can't find a battery.</t>
+  </si>
+  <si>
+    <t>2014-04-16</t>
+  </si>
+  <si>
+    <t>Poor battery, wish I saw these reviews before buying.</t>
+  </si>
+  <si>
+    <t>Out of the package, everything seemed great. But 6 months later, I can only get 45 seconds of use after charging all night. I guess you get what you pay for.</t>
+  </si>
+  <si>
+    <t>2014-04-20</t>
+  </si>
+  <si>
+    <t>VERY POOR BATTERY LIFE</t>
+  </si>
+  <si>
+    <t>After a month of use. the battery no longer holds a charge. No replacement batteries are available through the manufacturer. Don;t purchase this product unless you need something disposable for temporary use. Otherwise, not worth the money.</t>
+  </si>
+  <si>
+    <t>2014-04-29</t>
+  </si>
+  <si>
+    <t>TERRIBLE BATTERY</t>
+  </si>
+  <si>
+    <t>Never holds a charge... Very disappointed with this product.. Hoping to get a replacement or my money back :(</t>
+  </si>
+  <si>
+    <t>Buy a better trimmer</t>
+  </si>
+  <si>
+    <t>You wake up in the morning. You have to get to work. You pull out your Remington PG 6020, and get half way across your face, when the battery dies.  "No problem," you think, "I'll just plug it in and finish the other half of my face."  You find the cord, plug it in, and see the green lights turn on. You turn the trimmer on, the green lights go out, the trimmer makes another last dying buzz and stops. You flip the switch off. The green lights come back on.  You sit at home, late for work, with half of your face shaved, hoping that it doesn't actually take the 14 hours to charge that was recommended to you when you called "800-736-4648, M-F, 8 – 4 central time".  But you'll never know how long it takes to charge, because the charging light never goes out.</t>
+  </si>
+  <si>
+    <t>2014-05-13</t>
+  </si>
+  <si>
+    <t>Very Disappointed!!!!</t>
+  </si>
+  <si>
+    <t>The kids and I bought this for my husband for his birthday. It seemed to work OK the first few times. Then after about a week it just stopped holding a charge. It literally lasts about a minute or 2? What a waste of money! Plus my husband is out of his gift. The kids feel bad they got him something that doesn't work. The only good thing about this product is the different attachments. But I guess it doesn't matter if the item doesn't work. Very disappointed!!</t>
+  </si>
+  <si>
+    <t>2014-05-14</t>
+  </si>
+  <si>
+    <t>Not a bad product</t>
+  </si>
+  <si>
+    <t>I like using this product because it's quick when I'm in a rush. I leave mine on a charger so I don't have battery issues that I have read in other reviews. The one problem I found was the large shaver head doesn't work. The motor runs, but the blade doesn't move. This happened about a couple weeks after I got it. That is disappointing because that's the one I would use the most. I am hoping to either get a replacement part or my money back.</t>
+  </si>
+  <si>
+    <t>2014-05-20</t>
+  </si>
+  <si>
+    <t>Worked fine when I purchased it...</t>
+  </si>
+  <si>
+    <t>... Until about 6 months in. Does not hold charge despite lighting up, or simply does not run anymore. Very disappointed, as it seemed to do the job immediately after purchase. Attachments are fine. For the price it was a steal, but not if you have to replace or discard due to mechanical deficiencies.</t>
+  </si>
+  <si>
+    <t>disapointed</t>
+  </si>
+  <si>
+    <t>Was happy at first with this product, until it wouldn't hold a charge anymore, even after being plugged in. I also noticed the blades are dull. I will not buy Remington again.</t>
+  </si>
+  <si>
+    <t>2014-06-25</t>
+  </si>
+  <si>
+    <t>The all-in-1 Grooming System works fair.</t>
+  </si>
+  <si>
+    <t>The all-in-1 Grooming System works fair. The only item I believe should be added is a cleaning brush. In addition, the speed of the trimmer is lower than expected. I would like to try another one, just like this one, to observe the speed. The system I have may have a faulty battery. I allowed the battery to charge for the suggested time, but I believe the battery power isn't functioning at maximum output.</t>
+  </si>
+  <si>
+    <t>2014-07-03</t>
+  </si>
+  <si>
+    <t>Terrible battery quality</t>
+  </si>
+  <si>
+    <t>This product worked well for the 5 minutes or so of charge that it initially held. However, after just the third use, the battery will only hold a charge for 10-20 SECONDS. This trimmer is basically useless now, and judging from past reviews, this is a fairly common problem.</t>
+  </si>
+  <si>
+    <t>2014-07-05</t>
+  </si>
+  <si>
+    <t>Best grooming kit I have ever used</t>
+  </si>
+  <si>
+    <t>I have been looking for something like this for years. Much better than any I have had in past. Powerful motor, great attachments and works like a charm. Price is terrific! Highly recommended. Thanks Remington</t>
+  </si>
+  <si>
+    <t>2014-07-23</t>
+  </si>
+  <si>
+    <t>Didn't shave anything</t>
+  </si>
+  <si>
+    <t>Took it out of the box yesterday, gave it a try, and the blade was weak. It barely shaved any hair off. I'm returning it today.</t>
+  </si>
+  <si>
+    <t>2014-08-09</t>
+  </si>
+  <si>
+    <t>Nice features but very poor battery life.</t>
+  </si>
+  <si>
+    <t>The trimmers have nice attachments however the battery doesn't hold enough life to trim half a beard. Hopefully there is something on the market with a little more shave time.</t>
+  </si>
+  <si>
+    <t>2014-08-31</t>
+  </si>
+  <si>
+    <t>Disappointing!</t>
+  </si>
+  <si>
+    <t>I bought this grooming system approximately 8 months ago and already it's not working properly. When the system is charged, it is not keeping the charge. I was very disappointed with the system.</t>
+  </si>
+  <si>
+    <t>2014-09-09</t>
+  </si>
+  <si>
+    <t>machine does not keep it's charge</t>
+  </si>
+  <si>
+    <t>The critical flaw with this product is the grossly underpowered motor, power adapter and/or battery. The motor of the device simply isn't strong enough to fight the resistance created by its own attachments that were designed for it. Only if you remove all attachments and look at the spinning metal knob will you realize that the product actually does try to do something, and does have and keeps a charge, but the motor isn't strong enough to move that knob while inside an attachment to do anything significant. The result is the moment you attempt to use even the default attachment, the knob isn't able to move the blades after around 4 seconds of use, and the device dies, even on a full charge.</t>
+  </si>
+  <si>
+    <t>2014-10-30</t>
+  </si>
+  <si>
+    <t>Won't hold charge</t>
+  </si>
+  <si>
+    <t>I really enjoyed this grooming kit but unfortunately it will no longer hold a charge. The battery dies after only a few seconds of use.</t>
+  </si>
+  <si>
+    <t>won't hold a charge</t>
+  </si>
+  <si>
+    <t>After being plugged in/charging for two days, this trimmer runs less than 30 seconds.</t>
+  </si>
+  <si>
+    <t>2014-11-10</t>
+  </si>
+  <si>
+    <t>PG-6020</t>
+  </si>
+  <si>
+    <t>Severely poor battery life. I was not able to use it one time before the battery died. Always on the go, I generally groom on my way out, in my car at red lights. Unfortunately I bought this with a gift card and don't have the receipt. No way can I recommend this product.</t>
+  </si>
+  <si>
+    <t>2014-12-11</t>
+  </si>
+  <si>
+    <t>Poor battery life</t>
+  </si>
+  <si>
+    <t>Before reading these reviews I thought that I was the only person with this problem. I have had this trimmer for about a year and when new it would hold a charge for maybe five minutes but now after using the trimmer for about 15 seconds or so the battery goes completely dead. I have to plug the unit in for about five minutes to complete my mustache trim.</t>
+  </si>
+  <si>
+    <t>2014-12-12</t>
+  </si>
+  <si>
+    <t>DO NOT BUY JUNK!</t>
+  </si>
+  <si>
+    <t>Purchased this trimmer a few months ago and its useless, battery will not hold a charge so I'm going back to the old way and use scissors.</t>
+  </si>
+  <si>
+    <t>The instructions indicate that you should charge the device for at least 12-14 hours before use, and trying to use it without doing that charge makes it clear why those instructions exist: The device will turn on for a second or two, then stop working. That's fine, so you charge it for a day and intend to use it the next day. The problem is, even if you give it up to 24 hours the longest the device will give you a shave for is about 4 seconds, enough time to remove one sideburn. Is this product a joke? I plugged it in at around 7:00 AM and attempted to use it at around 7:00 AM the following morning. The device cut one of my sideburns, and just turned off. Thankfully I kept my old trimmer so I could just use that one, but this product really seems like you would buy it to play a cruel joke on someone, to see them come into work with half their mustache trimmed or something like that. The critical flaw with this product is the grossly underpowered motor, power adapter and/or battery. The motor of the device simply isn't strong enough to fight the resistance created by its own attachments that were designed for it. Only if you remove all attachments and look at the spinning metal knob will you realize that the product actually does try to do something, and does have and keeps a charge, but the motor isn't strong enough to move that knob while inside an attachment to do anything significant. The result is the moment you attempt to use even the default attachment, the knob isn't able to move the blades after around 4 seconds of use, and the device dies, even on a full charge.</t>
+  </si>
+  <si>
+    <t>2011-08-04</t>
+  </si>
+  <si>
+    <t>I bought this from a local grocery store as a replacement for multiple tools I used to use that have either stopped working completely, or stopped functioning correctly. The clippers:This is the main reason I purchased this, and while the clippers without the guard work well, the guard has absolutely no merit on the product itself 'cause it just doesnt work. I cut my own hair, figured this would work and it did but there is no guide as to what length each setting means other than 1,2,3,4,5,etc.. The nose trimmer:For me, this doesn't work at all its nearly too large to actually fit inside my nose and the angles I have to put it at are just obsurd. The Shaver:This is one of the main reasons I purchased this product as my old remmington shaver stopped working the way it should after a good 10+ years. It worked well for some of my hair, but the closeness of the shave is nowhere near that of a blade razor or my old remmington electric shaver that I had prior to this. I've had the product not very long and now the shaver doesn't work at all. I tried following the industructions to clean it and it just doesn't work. Product as a whole:I brought the product home, unpackaged it and read the instructions before doing anything with it. It said to charge it for a while before use so I plugged it in. Problem is the plug wouldn't stay inside the shaver unit itself long enough to charge the batteries or so I thought. I cracked open the unit (no screws hold it together), and noticed that the ground wire on the charging circut board the entire solder joint had broken apart. So if the solder point wasnt touching the circut board, it wasnt charging (no light).. I fixed this myself bu melting the solder, and adding a little bit more. It now charges, but not every consumer is going to own or know how to solder something together. The motor when no attachments are on it seems very strong, but once you add an attachment it seems to get very weak which could result in hair being pulled out instead of cut. I've only owned this unit for about 7 days now and I've already gone through these issues with the product. There are only a few ways i'd recommend this product and these are as follows: 1. you know how to solder (by the other reviews about no charging taking place, seems like you'll have to).2. you throw away the guides, the nose trimmer, the foil shaver, and everything else but the clipper portion.3. you intend to use it for nothing more than shaving your long haired animals. If all 3 of the above are true, then by all means spend the money but otherwise do yourself a favor and buy a better product if you have the money.</t>
+  </si>
+  <si>
+    <t>I went in looking for 2 products. One for nose and one to trim off my beard so I could shave.I found this one for a little more than a nose hair trimmer costs, and it seemed to say it did so much more.I've used the hair and beard trimmer guides, the shaver, nose hair cutter. The only adapter I haven't used is the rocking detailer thing.All the parts have worked great for me. I'm working up the nerve to try the hair trimmer for an at home haircut.The number guides on the guards make great sense to me and work well.</t>
+  </si>
+  <si>
+    <t>I have always been satisfied with Remington's products. However, this one is my favorite! It’s great for on the go touch up’s and for all body parts! Thanks Remington!</t>
+  </si>
+  <si>
+    <t>This product really takes care of everything, whether I'm going for the last minute buzz cut or just touching up this chargeable trimmer is very user friendly. I love the quickly swappable pieces and carrying case. I wish there was a spot for the charging cord in the case. Excellent value.</t>
+  </si>
+  <si>
+    <t>This product is well worth the money. Compared to other shavers i've had in the past this one is much more convenient. The multiple changeable heads and case is nice. The only downside i've seen is that some of the heads don't turn into place. This had no effect on the functionality however.</t>
+  </si>
+  <si>
+    <t>I received this all in one system on Wednesday and was finally able to use it over the weekend. I have used a number of other trimmers/groomers in the past so that gives me a good basis for comparison here. First off, I was glad to see that my device was shipped to me charged. This is a benefit for anyone who doesn't want to waste time charging the product for 12 hours before they can use the item they just purchased. I don't know if they all ship charged or I just got lucky, but that was a plus in my book. The carrying case included that contains all the variety of heads and bells &amp; whistles was a great touch, although I'm not sure how often I will bring this product on trips due to the nature of its use cases. The product itself performs admirably in its core roles, and is definitely precise enough for more intimate operations. I haven't run a full charge down yet, so I can't comment on battery life or durability specifically, but it appears to have a strong battery shelf life and to be fairly robust as a whole. If I was in the market again I would lean towards purchasing this set.</t>
+  </si>
+  <si>
+    <t>2011-12-12</t>
+  </si>
+  <si>
+    <t>Received this product as a gift. Charged it according to the instruction manual. When turned on, it performed as if it needed charged. I discharged the unit completely, then charged it again per the instruction manual and still it does not perform as if it is charged. This is the only Remington product that I have been dissatisfied with in the past 25 years of using Remington products.</t>
+  </si>
+  <si>
+    <t>2012-02-13</t>
+  </si>
+  <si>
+    <t>Have used it for 2 weeks--first complaint is that pieces do not fit into 'case' securely--case itself is very flimsy--not all pieces fit in proper allotted spaces.I have not had problems as others seem to have with charging and length of times in between charging.I have tried all the pieces and have not had luck with hair clipper and beard clipper--I may be using them wrong but have no way to tell as instructions don't help.I will use it as a nose, eyebrow and ear trimmer, possibly for mustache trimmer but as far as beard and hair I either will have to experiment more or just use a good old soap, water and razor</t>
+  </si>
+  <si>
+    <t>2012-05-20</t>
+  </si>
+  <si>
+    <t>2012-06-12</t>
+  </si>
+  <si>
+    <t>THEEE Best!!!</t>
+  </si>
+  <si>
+    <t>My husband absolutely LOVES this product! He say's it's the closest shave he has gotten from any of his past Remington trimmers/clippers!</t>
+  </si>
+  <si>
+    <t>2012-06-13</t>
+  </si>
+  <si>
+    <t>Bought this because I have a similar item from another company at home and forgot it on a three week trip. I use them to shave my head and chest and this could not do either. I don't imagine it would work for facial hair either seeing as mine would barely cut any hair. I pushed through and managed to get a very uneven cut on my head. I thought maybe they were having a rough time with my head hair so I tried using it on my chest hair and that was even worse. Had to go buy another set of clippers just to finish the job. Leaves tons of hair behind and will not cut closs to the skin at all. What a waste of money. Horrible product. On another note it took me nearly 20 minutes to get a somewhat even cut on my head and I never had a problem with the battery. (not that a battery does any good when the clippers don't work)</t>
+  </si>
+  <si>
+    <t>2012-10-24</t>
+  </si>
+  <si>
+    <t>Bought this 6 months ago and it's junk. Battery would hold a charge to finish the job and won't run when plugged in. Now 6 months later the battery won't even take a charge.Don't waste your money on this PG</t>
+  </si>
+  <si>
+    <t>2013-02-03</t>
+  </si>
+  <si>
+    <t>2013-02-27</t>
+  </si>
+  <si>
+    <t>my sister bought this for me.bab battery life and for some reason the main part that cuts the hair broke..it just dont move.!! propably the worst i ve ever had.</t>
+  </si>
+  <si>
+    <t>2013-06-16</t>
+  </si>
+  <si>
+    <t>The product itself is fine. It trims neatly and well, with lots of different attachments. However, it does not hold a charge to save it's life. You are lucky to get a minute or two of shaving out of it after several hours of charging. If you want to do any measurable shave out of it, you need to leave it on the charger overnight, and MAYBE it will last 5 mins. Do not suggest buying.</t>
+  </si>
+  <si>
+    <t>DO NOT PURCHASE THIS PRODUCT. I purchased a Remington1 all-in-one grooming system about a month ago and it is the worst grooming kit I have ever purchased. The shaver runs off of battery only, can't be used while plugged into an electrical outlet. The batter barley lasts long enough to shave my head or trim my beard. I do not recommend this product.</t>
+  </si>
+  <si>
+    <t>Bought the All in 1 Grooming system and was extremely disappointed with the product.Can bearly manage one beard trimming before the battery is complete dead.</t>
+  </si>
+  <si>
+    <t>2013-11-23</t>
+  </si>
+  <si>
+    <t>2013-11-30</t>
+  </si>
+  <si>
+    <t>Couldn't Beat it for the Price</t>
+  </si>
+  <si>
+    <t>Does what it says it will do. My husband really liked it and the base holds everything well. And I really could not beat it for the price. No reason to spend more when these tools do what they do.</t>
+  </si>
+  <si>
+    <t>Pros: As a grooming tool I liked all of the attachments and it fits well in your hand. It does a good job at doing what it was made for. Cons: The stand it comes in does not function well unless your just into displaying your stuff. The cord comes around the front of the stand in order to plug into the shaver as it barely sits in it's cradle. The battery gave out six months into use. I could live with the rest of the shortcomings of this unit but not this one. I would not recommend this product.</t>
+  </si>
+  <si>
+    <t>I purchased this product to replace an old trimmer made by a competitor that had served me for years. I selected this model because it had a greater variety of attachments than comparable products, and I figured it would be versatile. Given that this is a low-cost product, my expectations were modest, but the product failed to meet even those modest expectations. As others pointed out, the battery life is the biggest drawback. Even when brand new and fully charged, the battery affords me a scant ten minutes of usage time. Normally, that wouldn't be a problem, since I can trim my beard in ten minutes. However, the blades on the unit are so dull that they continuously jam and clog, even on the thinnest parts of my beard, resulting in painful pulling. I have to make at least six or seven passes over each part of my beard just to get a basic trim. The result is that I can only ever trim about a third of my beard with this product, then I end up finishing off with scissors and a comb. Overall, this is one of the poorest-performing consumer products I've ever purchased. I strongly advise against purchasing it.</t>
+  </si>
+  <si>
+    <t>2013-12-07</t>
+  </si>
+  <si>
+    <t>Great Buy</t>
+  </si>
+  <si>
+    <t>Compact size makes for easy storage. Long lasting battery.</t>
+  </si>
+  <si>
+    <t>The power delivery system on my clipper fails and the battery life is nonexistent. The clipper will not work without a power cord and even with a power cord it must be charged for about an hour before use. Then, when it does work, the power drains so quickly that it renders the clipper useless. I had presumed that it was just my clipper that was defective, but I have read countless reviews by others who had the same problem. I did not expect much from this inexpensive product, but I expected more than what it offered me. This product makes a good target for shooting practice.</t>
+  </si>
+  <si>
+    <t>2013-12-28</t>
+  </si>
+  <si>
+    <t>Great Groomer</t>
+  </si>
+  <si>
+    <t>Nice purchase. My son really likes it. Many attachments featured. A lot of bang for your buck!</t>
+  </si>
+  <si>
+    <t>Perfect grooming</t>
+  </si>
+  <si>
+    <t>Everything you need for a perfect groom also a great product for a reasonable price a must have item highly recommended</t>
+  </si>
+  <si>
+    <t>Given as gift</t>
+  </si>
+  <si>
+    <t>Have not heard any complaints. It was given as a gift.</t>
+  </si>
+  <si>
+    <t>Do not buy</t>
+  </si>
+  <si>
+    <t>It doesn't trim anything. Don't waste your money. I would say good value but it doesn't do anything.</t>
+  </si>
+  <si>
+    <t>Great Gift</t>
+  </si>
+  <si>
+    <t>It was a gift for my boyfriend. I am always complaining about his facial hair not being kept. Ever since I purchased the grooming set, we no longer have this issue. He loves the set and uses it all the time. The stand is a big plus. The stand holds all the attachment in place so he does not have to worry about losing anything.</t>
+  </si>
+  <si>
+    <t>2014-02-27</t>
+  </si>
+  <si>
+    <t>Awesome Puchase</t>
+  </si>
+  <si>
+    <t>Well worth it! The price was great &amp; the trimmer is AWESOME! Very happy with our purchase!</t>
+  </si>
+  <si>
+    <t>I used this product for 2 years and the battery died - it would run only for 30 sec after charging for 24 hrs.I tried to find a replacement battery but could not.It's kind of sad to throw away a working device because you can't find a battery.</t>
+  </si>
+  <si>
+    <t>2014-04-15</t>
+  </si>
+  <si>
+    <t>2014-04-21</t>
+  </si>
+  <si>
+    <t>Not impressed</t>
+  </si>
+  <si>
+    <t>Doesn't cut close enough to the skin and dies too fast. My boyfriend only used it to trim his beard not for shaving</t>
+  </si>
+  <si>
+    <t>You wake up in the morning. You have to get to work. You pull out your Remington PG 6020, and get half way across your face, when the battery dies. "No problem," you think, "I'll just plug it in and finish the other half of my face." You find the cord, plug it in, and see the green lights turn on.You turn the trimmer on, the green lights go out, the trimmer makes another last dying buzz and stops.You flip the switch off.The green lights come back on. You sit at home, late for work, with half of your face shaved, hoping that it doesn't actually take the 14 hours to charge that was recommended to you when you called "800-736-4648, M-F, 8 – 4 central time". But you'll never know how long it takes to charge, because the charging light never goes out.</t>
+  </si>
+  <si>
+    <t>2014-05-15</t>
+  </si>
+  <si>
+    <t>Doesn't hold charge</t>
+  </si>
+  <si>
+    <t>doesn't charge quickly or hold a charge. no power.</t>
+  </si>
+  <si>
+    <t>2014-05-19</t>
+  </si>
+  <si>
+    <t>2014-06-20</t>
+  </si>
+  <si>
+    <t>Great Investment</t>
+  </si>
+  <si>
+    <t>My husband loved this, for Fathers Day. He can't stop using it. I'm really glad I purchased it for him.</t>
+  </si>
+  <si>
+    <t>2014-06-21</t>
+  </si>
+  <si>
+    <t>Great Father's Day gift</t>
+  </si>
+  <si>
+    <t>I bought this product for Father's Day! He loves it</t>
+  </si>
+  <si>
+    <t>The all-in-1 Grooming System works fair. The only item I believe should be added is a cleaning brush.In addition, the speed of the trimmer is lower than expected.I would like to try another one, just like this one, to observe the speed.The system I have may have a faulty battery. I allowed the battery to charge for the suggested time, but I believe the battery power isn’t functioning at maximum output.</t>
+  </si>
+  <si>
+    <t>2014-07-02</t>
+  </si>
+  <si>
+    <t>2014-08-08</t>
+  </si>
+  <si>
+    <t>2014-11-09</t>
   </si>
 </sst>
 </file>
@@ -1454,10 +2513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E136"/>
+  <dimension ref="A1:E333"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="B140" sqref="B140"/>
+    <sheetView tabSelected="1" topLeftCell="A216" workbookViewId="0">
+      <selection activeCell="J231" sqref="J231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3542,12 +4601,12 @@
         <v>336</v>
       </c>
     </row>
-    <row r="123" spans="1:5">
+    <row r="123" spans="1:5" s="2" customFormat="1">
       <c r="A123" s="2" t="s">
         <v>182</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>337</v>
+        <v>358</v>
       </c>
       <c r="C123" s="3">
         <v>1</v>
@@ -3559,12 +4618,12 @@
         <v>339</v>
       </c>
     </row>
-    <row r="124" spans="1:5">
+    <row r="124" spans="1:5" s="2" customFormat="1">
       <c r="A124" s="2" t="s">
         <v>340</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>337</v>
+        <v>358</v>
       </c>
       <c r="C124" s="3">
         <v>1</v>
@@ -3576,12 +4635,12 @@
         <v>342</v>
       </c>
     </row>
-    <row r="125" spans="1:5">
+    <row r="125" spans="1:5" s="2" customFormat="1">
       <c r="A125" s="2" t="s">
-        <v>343</v>
+        <v>211</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>337</v>
+        <v>358</v>
       </c>
       <c r="C125" s="3">
         <v>2</v>
@@ -3593,12 +4652,12 @@
         <v>345</v>
       </c>
     </row>
-    <row r="126" spans="1:5">
+    <row r="126" spans="1:5" s="2" customFormat="1">
       <c r="A126" s="2" t="s">
         <v>346</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>337</v>
+        <v>358</v>
       </c>
       <c r="C126" s="3">
         <v>1</v>
@@ -3610,12 +4669,12 @@
         <v>348</v>
       </c>
     </row>
-    <row r="127" spans="1:5">
+    <row r="127" spans="1:5" s="2" customFormat="1">
       <c r="A127" s="2" t="s">
-        <v>349</v>
+        <v>359</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>337</v>
+        <v>358</v>
       </c>
       <c r="C127" s="3">
         <v>1</v>
@@ -3627,12 +4686,12 @@
         <v>351</v>
       </c>
     </row>
-    <row r="128" spans="1:5">
+    <row r="128" spans="1:5" s="2" customFormat="1">
       <c r="A128" s="2" t="s">
         <v>352</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>337</v>
+        <v>358</v>
       </c>
       <c r="C128" s="3">
         <v>2</v>
@@ -3644,12 +4703,12 @@
         <v>354</v>
       </c>
     </row>
-    <row r="129" spans="1:5">
+    <row r="129" spans="1:5" s="2" customFormat="1">
       <c r="A129" s="2" t="s">
-        <v>355</v>
+        <v>360</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>337</v>
+        <v>358</v>
       </c>
       <c r="C129" s="3">
         <v>1</v>
@@ -3663,120 +4722,3469 @@
     </row>
     <row r="130" spans="1:5" s="2" customFormat="1">
       <c r="A130" s="2" t="s">
-        <v>182</v>
+        <v>361</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>358</v>
+        <v>337</v>
       </c>
       <c r="C130" s="3">
         <v>1</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>338</v>
+        <v>362</v>
       </c>
       <c r="E130" s="2" t="s">
-        <v>339</v>
+        <v>363</v>
       </c>
     </row>
     <row r="131" spans="1:5" s="2" customFormat="1">
       <c r="A131" s="2" t="s">
-        <v>340</v>
+        <v>364</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>358</v>
+        <v>337</v>
       </c>
       <c r="C131" s="3">
         <v>1</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>341</v>
+        <v>365</v>
       </c>
       <c r="E131" s="2" t="s">
-        <v>342</v>
+        <v>366</v>
       </c>
     </row>
     <row r="132" spans="1:5" s="2" customFormat="1">
       <c r="A132" s="2" t="s">
-        <v>211</v>
+        <v>367</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>358</v>
+        <v>337</v>
       </c>
       <c r="C132" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>344</v>
+        <v>368</v>
       </c>
       <c r="E132" s="2" t="s">
-        <v>345</v>
+        <v>369</v>
       </c>
     </row>
     <row r="133" spans="1:5" s="2" customFormat="1">
       <c r="A133" s="2" t="s">
-        <v>346</v>
+        <v>370</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>358</v>
+        <v>337</v>
       </c>
       <c r="C133" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>347</v>
+        <v>371</v>
       </c>
       <c r="E133" s="2" t="s">
-        <v>348</v>
+        <v>372</v>
       </c>
     </row>
     <row r="134" spans="1:5" s="2" customFormat="1">
       <c r="A134" s="2" t="s">
-        <v>359</v>
+        <v>373</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>358</v>
+        <v>337</v>
       </c>
       <c r="C134" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>350</v>
+        <v>374</v>
       </c>
       <c r="E134" s="2" t="s">
-        <v>351</v>
+        <v>375</v>
       </c>
     </row>
     <row r="135" spans="1:5" s="2" customFormat="1">
       <c r="A135" s="2" t="s">
-        <v>352</v>
+        <v>376</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>358</v>
+        <v>337</v>
       </c>
       <c r="C135" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>353</v>
+        <v>377</v>
       </c>
       <c r="E135" s="2" t="s">
-        <v>354</v>
+        <v>378</v>
       </c>
     </row>
     <row r="136" spans="1:5" s="2" customFormat="1">
       <c r="A136" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C136" s="3">
+        <v>5</v>
+      </c>
+      <c r="D136" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="E136" s="2" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" s="2" customFormat="1">
+      <c r="A137" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C137" s="3">
+        <v>5</v>
+      </c>
+      <c r="D137" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="E137" s="2" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" s="2" customFormat="1">
+      <c r="A138" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C138" s="3">
+        <v>5</v>
+      </c>
+      <c r="D138" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="E138" s="2" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" s="2" customFormat="1">
+      <c r="A139" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C139" s="3">
+        <v>4</v>
+      </c>
+      <c r="D139" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="E139" s="2" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" s="2" customFormat="1">
+      <c r="A140" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C140" s="3">
+        <v>4</v>
+      </c>
+      <c r="D140" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="E140" s="2" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" s="2" customFormat="1">
+      <c r="A141" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C141" s="3">
+        <v>3</v>
+      </c>
+      <c r="D141" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="E141" s="2" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" s="2" customFormat="1">
+      <c r="A142" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C142" s="3">
+        <v>1</v>
+      </c>
+      <c r="D142" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="E142" s="2" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" s="2" customFormat="1">
+      <c r="A143" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C143" s="3">
+        <v>2</v>
+      </c>
+      <c r="D143" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="E143" s="2" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" s="2" customFormat="1">
+      <c r="A144" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C144" s="3">
+        <v>1</v>
+      </c>
+      <c r="D144" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="E144" s="2" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" s="2" customFormat="1">
+      <c r="A145" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C145" s="3">
+        <v>1</v>
+      </c>
+      <c r="D145" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="E145" s="2" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" s="2" customFormat="1">
+      <c r="A146" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C146" s="3">
+        <v>3</v>
+      </c>
+      <c r="D146" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="E146" s="2" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" s="2" customFormat="1">
+      <c r="A147" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C147" s="3">
+        <v>1</v>
+      </c>
+      <c r="D147" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="E147" s="2" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" s="2" customFormat="1">
+      <c r="A148" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C148" s="3">
+        <v>1</v>
+      </c>
+      <c r="D148" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="E148" s="2" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" s="2" customFormat="1">
+      <c r="A149" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C149" s="3">
+        <v>1</v>
+      </c>
+      <c r="D149" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="E149" s="2" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" s="2" customFormat="1">
+      <c r="A150" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C150" s="3">
+        <v>4</v>
+      </c>
+      <c r="D150" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="E150" s="2" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" s="2" customFormat="1">
+      <c r="A151" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C151" s="3">
+        <v>1</v>
+      </c>
+      <c r="D151" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="E151" s="2" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" s="2" customFormat="1">
+      <c r="A152" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C152" s="3">
+        <v>5</v>
+      </c>
+      <c r="D152" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="E152" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" s="2" customFormat="1">
+      <c r="A153" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C153" s="3">
+        <v>1</v>
+      </c>
+      <c r="D153" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="E153" s="2" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" s="2" customFormat="1">
+      <c r="A154" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C154" s="3">
+        <v>1</v>
+      </c>
+      <c r="D154" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="E154" s="2" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" s="2" customFormat="1">
+      <c r="A155" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C155" s="3">
+        <v>1</v>
+      </c>
+      <c r="D155" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="E155" s="2" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" s="2" customFormat="1">
+      <c r="A156" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C156" s="3">
+        <v>4</v>
+      </c>
+      <c r="D156" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="E156" s="2" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" s="2" customFormat="1">
+      <c r="A157" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C157" s="3">
+        <v>2</v>
+      </c>
+      <c r="D157" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="E157" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" s="2" customFormat="1">
+      <c r="A158" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C158" s="3">
+        <v>3</v>
+      </c>
+      <c r="D158" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="E158" s="2" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" s="2" customFormat="1">
+      <c r="A159" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C159" s="3">
+        <v>1</v>
+      </c>
+      <c r="D159" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="E159" s="2" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" s="2" customFormat="1">
+      <c r="A160" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C160" s="3">
+        <v>1</v>
+      </c>
+      <c r="D160" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="E160" s="2" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" s="2" customFormat="1">
+      <c r="A161" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C161" s="3">
+        <v>3</v>
+      </c>
+      <c r="D161" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="E161" s="2" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" s="2" customFormat="1">
+      <c r="A162" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C162" s="3">
+        <v>1</v>
+      </c>
+      <c r="D162" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="E162" s="2" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" s="2" customFormat="1">
+      <c r="A163" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C163" s="3">
+        <v>4</v>
+      </c>
+      <c r="D163" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="E163" s="2" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" s="2" customFormat="1">
+      <c r="A164" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C164" s="3">
+        <v>5</v>
+      </c>
+      <c r="D164" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="E164" s="2" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" s="2" customFormat="1">
+      <c r="A165" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="B165" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C165" s="3">
+        <v>2</v>
+      </c>
+      <c r="D165" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="E165" s="2" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" s="2" customFormat="1">
+      <c r="A166" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C166" s="3">
+        <v>1</v>
+      </c>
+      <c r="D166" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="E166" s="2" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" s="2" customFormat="1">
+      <c r="A167" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C167" s="3">
+        <v>5</v>
+      </c>
+      <c r="D167" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="E167" s="2" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" s="2" customFormat="1">
+      <c r="A168" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="B168" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C168" s="3">
+        <v>1</v>
+      </c>
+      <c r="D168" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E168" s="2" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" s="2" customFormat="1">
+      <c r="A169" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C169" s="3">
+        <v>2</v>
+      </c>
+      <c r="D169" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="E169" s="2" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" s="2" customFormat="1">
+      <c r="A170" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C170" s="3">
+        <v>1</v>
+      </c>
+      <c r="D170" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="E170" s="2" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" s="2" customFormat="1">
+      <c r="A171" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C171" s="3">
+        <v>1</v>
+      </c>
+      <c r="D171" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="E171" s="2" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" s="2" customFormat="1">
+      <c r="A172" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="B172" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C172" s="3">
+        <v>1</v>
+      </c>
+      <c r="D172" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="E172" s="2" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" s="2" customFormat="1">
+      <c r="A173" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C173" s="3">
+        <v>1</v>
+      </c>
+      <c r="D173" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="E173" s="2" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" s="2" customFormat="1">
+      <c r="A174" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="B174" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C174" s="3">
+        <v>1</v>
+      </c>
+      <c r="D174" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="E174" s="2" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" s="2" customFormat="1">
+      <c r="A175" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="B175" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C175" s="3">
+        <v>2</v>
+      </c>
+      <c r="D175" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="E175" s="2" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" s="2" customFormat="1">
+      <c r="A176" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="B176" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C176" s="3">
+        <v>1</v>
+      </c>
+      <c r="D176" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="E176" s="2" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" s="2" customFormat="1">
+      <c r="A177" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C177" s="3">
+        <v>1</v>
+      </c>
+      <c r="D177" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="E177" s="2" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" s="2" customFormat="1">
+      <c r="A178" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C178" s="3">
+        <v>2</v>
+      </c>
+      <c r="D178" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="E178" s="2" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" s="2" customFormat="1">
+      <c r="A179" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C179" s="3">
+        <v>5</v>
+      </c>
+      <c r="D179" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="E179" s="2" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" s="2" customFormat="1">
+      <c r="A180" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="B180" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C180" s="3">
+        <v>1</v>
+      </c>
+      <c r="D180" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="E180" s="2" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" s="2" customFormat="1">
+      <c r="A181" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C181" s="3">
+        <v>1</v>
+      </c>
+      <c r="D181" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="E181" s="2" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" s="2" customFormat="1">
+      <c r="A182" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="B182" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C182" s="3">
+        <v>1</v>
+      </c>
+      <c r="D182" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E182" s="2" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" s="2" customFormat="1">
+      <c r="A183" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C183" s="3">
+        <v>4</v>
+      </c>
+      <c r="D183" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E183" s="2" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" s="2" customFormat="1">
+      <c r="A184" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="B184" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C184" s="3">
+        <v>5</v>
+      </c>
+      <c r="D184" s="2" t="s">
+        <v>518</v>
+      </c>
+      <c r="E184" s="2" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" s="2" customFormat="1">
+      <c r="A185" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="B185" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C185" s="3">
+        <v>5</v>
+      </c>
+      <c r="D185" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="E185" s="2" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" s="2" customFormat="1">
+      <c r="A186" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="B186" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C186" s="3">
+        <v>1</v>
+      </c>
+      <c r="D186" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="E186" s="2" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" s="2" customFormat="1">
+      <c r="A187" s="2" t="s">
+        <v>526</v>
+      </c>
+      <c r="B187" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C187" s="3">
+        <v>1</v>
+      </c>
+      <c r="D187" s="2" t="s">
+        <v>527</v>
+      </c>
+      <c r="E187" s="2" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" s="2" customFormat="1">
+      <c r="A188" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="B188" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C188" s="3">
+        <v>1</v>
+      </c>
+      <c r="D188" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E188" s="2" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" s="2" customFormat="1">
+      <c r="A189" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="B189" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C189" s="3">
+        <v>2</v>
+      </c>
+      <c r="D189" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="E189" s="2" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" s="2" customFormat="1">
+      <c r="A190" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="B190" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C190" s="3">
+        <v>1</v>
+      </c>
+      <c r="D190" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="E190" s="2" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" s="2" customFormat="1">
+      <c r="A191" s="2" t="s">
+        <v>537</v>
+      </c>
+      <c r="B191" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C191" s="3">
+        <v>1</v>
+      </c>
+      <c r="D191" s="2" t="s">
+        <v>538</v>
+      </c>
+      <c r="E191" s="2" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" s="2" customFormat="1">
+      <c r="A192" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="B192" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C192" s="3">
+        <v>4</v>
+      </c>
+      <c r="D192" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="E192" s="2" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" s="2" customFormat="1">
+      <c r="A193" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="B193" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C193" s="3">
+        <v>1</v>
+      </c>
+      <c r="D193" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="E193" s="2" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" s="2" customFormat="1">
+      <c r="A194" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B194" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C194" s="3">
+        <v>2</v>
+      </c>
+      <c r="D194" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="E194" s="2" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" s="2" customFormat="1">
+      <c r="A195" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B195" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C195" s="3">
+        <v>1</v>
+      </c>
+      <c r="D195" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="E195" s="2" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" s="2" customFormat="1">
+      <c r="A196" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="B196" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C196" s="3">
+        <v>5</v>
+      </c>
+      <c r="D196" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="E196" s="2" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" s="2" customFormat="1">
+      <c r="A197" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="B197" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C197" s="3">
+        <v>4</v>
+      </c>
+      <c r="D197" s="2" t="s">
+        <v>554</v>
+      </c>
+      <c r="E197" s="2" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" s="2" customFormat="1">
+      <c r="A198" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="B198" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C198" s="3">
+        <v>2</v>
+      </c>
+      <c r="D198" s="2" t="s">
+        <v>557</v>
+      </c>
+      <c r="E198" s="2" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" s="2" customFormat="1">
+      <c r="A199" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="B199" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C199" s="3">
+        <v>5</v>
+      </c>
+      <c r="D199" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="E199" s="2" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" s="2" customFormat="1">
+      <c r="A200" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="B200" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C200" s="3">
+        <v>3</v>
+      </c>
+      <c r="D200" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="E200" s="2" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" s="2" customFormat="1">
+      <c r="A201" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="B201" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C201" s="3">
+        <v>4</v>
+      </c>
+      <c r="D201" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="E201" s="2" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" s="2" customFormat="1">
+      <c r="A202" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="B202" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C202" s="3">
+        <v>2</v>
+      </c>
+      <c r="D202" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="E202" s="2" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" s="2" customFormat="1">
+      <c r="A203" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="B203" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C203" s="3">
+        <v>5</v>
+      </c>
+      <c r="D203" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="E203" s="2" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" s="2" customFormat="1">
+      <c r="A204" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="B204" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C204" s="3">
+        <v>3</v>
+      </c>
+      <c r="D204" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="E204" s="2" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" s="2" customFormat="1">
+      <c r="A205" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="B205" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C205" s="3">
+        <v>1</v>
+      </c>
+      <c r="D205" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="E205" s="2" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" s="2" customFormat="1">
+      <c r="A206" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="B206" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C206" s="3">
+        <v>1</v>
+      </c>
+      <c r="D206" s="2" t="s">
+        <v>581</v>
+      </c>
+      <c r="E206" s="2" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" s="2" customFormat="1">
+      <c r="A207" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="B207" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C207" s="3">
+        <v>1</v>
+      </c>
+      <c r="D207" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="E207" s="2" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" s="2" customFormat="1">
+      <c r="A208" s="2" t="s">
+        <v>586</v>
+      </c>
+      <c r="B208" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C208" s="3">
+        <v>1</v>
+      </c>
+      <c r="D208" s="2" t="s">
+        <v>587</v>
+      </c>
+      <c r="E208" s="2" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" s="2" customFormat="1">
+      <c r="A209" s="2" t="s">
+        <v>589</v>
+      </c>
+      <c r="B209" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C209" s="3">
+        <v>1</v>
+      </c>
+      <c r="D209" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="E209" s="2" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" s="2" customFormat="1">
+      <c r="A210" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="B210" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C210" s="3">
+        <v>1</v>
+      </c>
+      <c r="D210" s="2" t="s">
+        <v>593</v>
+      </c>
+      <c r="E210" s="2" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" s="2" customFormat="1">
+      <c r="A211" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B211" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C211" s="3">
+        <v>1</v>
+      </c>
+      <c r="D211" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="E211" s="2" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" s="2" customFormat="1">
+      <c r="A212" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="B212" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C212" s="3">
+        <v>1</v>
+      </c>
+      <c r="D212" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="E212" s="2" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" s="2" customFormat="1">
+      <c r="A213" s="2" t="s">
+        <v>600</v>
+      </c>
+      <c r="B213" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C213" s="3">
+        <v>3</v>
+      </c>
+      <c r="D213" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="E213" s="2" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" s="2" customFormat="1">
+      <c r="A214" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="B214" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C214" s="3">
+        <v>2</v>
+      </c>
+      <c r="D214" s="2" t="s">
+        <v>604</v>
+      </c>
+      <c r="E214" s="2" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" s="2" customFormat="1">
+      <c r="A215" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B215" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C215" s="3">
+        <v>1</v>
+      </c>
+      <c r="D215" s="2" t="s">
+        <v>606</v>
+      </c>
+      <c r="E215" s="2" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" s="2" customFormat="1">
+      <c r="A216" s="2" t="s">
+        <v>608</v>
+      </c>
+      <c r="B216" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C216" s="3">
+        <v>3</v>
+      </c>
+      <c r="D216" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="E216" s="2" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" s="2" customFormat="1">
+      <c r="A217" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="B217" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C217" s="3">
+        <v>1</v>
+      </c>
+      <c r="D217" s="2" t="s">
+        <v>612</v>
+      </c>
+      <c r="E217" s="2" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" s="2" customFormat="1">
+      <c r="A218" s="2" t="s">
+        <v>614</v>
+      </c>
+      <c r="B218" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C218" s="3">
+        <v>5</v>
+      </c>
+      <c r="D218" s="2" t="s">
+        <v>615</v>
+      </c>
+      <c r="E218" s="2" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" s="2" customFormat="1">
+      <c r="A219" s="2" t="s">
+        <v>617</v>
+      </c>
+      <c r="B219" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C219" s="3">
+        <v>1</v>
+      </c>
+      <c r="D219" s="2" t="s">
+        <v>618</v>
+      </c>
+      <c r="E219" s="2" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" s="2" customFormat="1">
+      <c r="A220" s="2" t="s">
+        <v>620</v>
+      </c>
+      <c r="B220" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C220" s="3">
+        <v>1</v>
+      </c>
+      <c r="D220" s="2" t="s">
+        <v>621</v>
+      </c>
+      <c r="E220" s="2" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" s="2" customFormat="1">
+      <c r="A221" s="2" t="s">
+        <v>623</v>
+      </c>
+      <c r="B221" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C221" s="3">
+        <v>1</v>
+      </c>
+      <c r="D221" s="2" t="s">
+        <v>624</v>
+      </c>
+      <c r="E221" s="2" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" s="2" customFormat="1">
+      <c r="A222" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="B222" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C222" s="3">
+        <v>1</v>
+      </c>
+      <c r="D222" s="2" t="s">
+        <v>627</v>
+      </c>
+      <c r="E222" s="2" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" s="2" customFormat="1">
+      <c r="A223" s="2" t="s">
+        <v>629</v>
+      </c>
+      <c r="B223" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C223" s="3">
+        <v>1</v>
+      </c>
+      <c r="D223" s="2" t="s">
+        <v>630</v>
+      </c>
+      <c r="E223" s="2" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" s="2" customFormat="1">
+      <c r="A224" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B224" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C224" s="3">
+        <v>1</v>
+      </c>
+      <c r="D224" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="E224" s="2" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" s="2" customFormat="1">
+      <c r="A225" s="2" t="s">
+        <v>634</v>
+      </c>
+      <c r="B225" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C225" s="3">
+        <v>1</v>
+      </c>
+      <c r="D225" s="2" t="s">
+        <v>635</v>
+      </c>
+      <c r="E225" s="2" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" s="2" customFormat="1">
+      <c r="A226" s="2" t="s">
+        <v>637</v>
+      </c>
+      <c r="B226" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C226" s="3">
+        <v>1</v>
+      </c>
+      <c r="D226" s="2" t="s">
+        <v>638</v>
+      </c>
+      <c r="E226" s="2" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" s="2" customFormat="1">
+      <c r="A227" s="2" t="s">
+        <v>640</v>
+      </c>
+      <c r="B227" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C227" s="3">
+        <v>1</v>
+      </c>
+      <c r="D227" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="E227" s="2" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" s="2" customFormat="1">
+      <c r="A228" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B228" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C228" s="3">
+        <v>1</v>
+      </c>
+      <c r="D228" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="E228" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" s="2" customFormat="1">
+      <c r="A229" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="B229" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C229" s="3">
+        <v>1</v>
+      </c>
+      <c r="D229" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="E229" s="2" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" s="2" customFormat="1">
+      <c r="A230" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="B230" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C230" s="3">
+        <v>2</v>
+      </c>
+      <c r="D230" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="E230" s="2" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" s="2" customFormat="1">
+      <c r="A231" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="B231" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C231" s="3">
+        <v>1</v>
+      </c>
+      <c r="D231" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="E231" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" s="2" customFormat="1">
+      <c r="A232" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="B232" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C232" s="3">
+        <v>1</v>
+      </c>
+      <c r="D232" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="E232" s="2" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" s="2" customFormat="1">
+      <c r="A233" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="B233" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C233" s="3">
+        <v>2</v>
+      </c>
+      <c r="D233" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="E233" s="2" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" s="2" customFormat="1">
+      <c r="A234" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B234" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C234" s="3">
+        <v>1</v>
+      </c>
+      <c r="D234" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="E234" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" s="2" customFormat="1">
+      <c r="A235" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="B235" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C235" s="3">
+        <v>1</v>
+      </c>
+      <c r="D235" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="E235" s="2" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" s="2" customFormat="1">
+      <c r="A236" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="B236" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C236" s="3">
+        <v>1</v>
+      </c>
+      <c r="D236" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="E236" s="2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" s="2" customFormat="1">
+      <c r="A237" s="2" t="s">
+        <v>644</v>
+      </c>
+      <c r="B237" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C237" s="3">
+        <v>1</v>
+      </c>
+      <c r="D237" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="E237" s="2" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" s="2" customFormat="1">
+      <c r="A238" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="B238" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C238" s="3">
+        <v>5</v>
+      </c>
+      <c r="D238" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="E238" s="2" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" s="2" customFormat="1">
+      <c r="A239" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="B239" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C239" s="3">
+        <v>5</v>
+      </c>
+      <c r="D239" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="E239" s="2" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" s="2" customFormat="1">
+      <c r="A240" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="B240" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C240" s="3">
+        <v>1</v>
+      </c>
+      <c r="D240" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="E240" s="2" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" s="2" customFormat="1">
+      <c r="A241" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="B241" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C241" s="3">
+        <v>5</v>
+      </c>
+      <c r="D241" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="E241" s="2" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" s="2" customFormat="1">
+      <c r="A242" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="B242" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C242" s="3">
+        <v>5</v>
+      </c>
+      <c r="D242" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="E242" s="2" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" s="2" customFormat="1">
+      <c r="A243" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="B243" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C243" s="3">
+        <v>5</v>
+      </c>
+      <c r="D243" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="E243" s="2" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" s="2" customFormat="1">
+      <c r="A244" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="B244" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C244" s="3">
+        <v>4</v>
+      </c>
+      <c r="D244" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="E244" s="2" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" s="2" customFormat="1">
+      <c r="A245" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="B245" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C245" s="3">
+        <v>4</v>
+      </c>
+      <c r="D245" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="E245" s="2" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5" s="2" customFormat="1">
+      <c r="A246" s="2" t="s">
+        <v>651</v>
+      </c>
+      <c r="B246" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C246" s="3">
+        <v>3</v>
+      </c>
+      <c r="D246" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="E246" s="2" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5" s="2" customFormat="1">
+      <c r="A247" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="B247" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C247" s="3">
+        <v>1</v>
+      </c>
+      <c r="D247" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="E247" s="2" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5" s="2" customFormat="1">
+      <c r="A248" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="B248" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C248" s="3">
+        <v>2</v>
+      </c>
+      <c r="D248" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="E248" s="2" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5" s="2" customFormat="1">
+      <c r="A249" s="2" t="s">
+        <v>653</v>
+      </c>
+      <c r="B249" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C249" s="3">
+        <v>1</v>
+      </c>
+      <c r="D249" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="E249" s="2" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5" s="2" customFormat="1">
+      <c r="A250" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="B250" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C250" s="3">
+        <v>1</v>
+      </c>
+      <c r="D250" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="E250" s="2" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5" s="2" customFormat="1">
+      <c r="A251" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="B251" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C251" s="3">
+        <v>3</v>
+      </c>
+      <c r="D251" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="E251" s="2" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5" s="2" customFormat="1">
+      <c r="A252" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="B252" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C252" s="3">
+        <v>1</v>
+      </c>
+      <c r="D252" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="E252" s="2" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5" s="2" customFormat="1">
+      <c r="A253" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="B253" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C253" s="3">
+        <v>1</v>
+      </c>
+      <c r="D253" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="E253" s="2" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5" s="2" customFormat="1">
+      <c r="A254" s="2" t="s">
+        <v>656</v>
+      </c>
+      <c r="B254" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C254" s="3">
+        <v>5</v>
+      </c>
+      <c r="D254" s="2" t="s">
+        <v>657</v>
+      </c>
+      <c r="E254" s="2" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5" s="2" customFormat="1">
+      <c r="A255" s="2" t="s">
+        <v>659</v>
+      </c>
+      <c r="B255" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C255" s="3">
+        <v>1</v>
+      </c>
+      <c r="D255" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="E255" s="2" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5" s="2" customFormat="1">
+      <c r="A256" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="B256" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C256" s="3">
+        <v>4</v>
+      </c>
+      <c r="D256" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="E256" s="2" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5" s="2" customFormat="1">
+      <c r="A257" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="B257" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C257" s="3">
+        <v>1</v>
+      </c>
+      <c r="D257" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="E257" s="2" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5" s="2" customFormat="1">
+      <c r="A258" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="B258" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C258" s="3">
+        <v>5</v>
+      </c>
+      <c r="D258" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="E258" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5" s="2" customFormat="1">
+      <c r="A259" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="B259" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C259" s="3">
+        <v>1</v>
+      </c>
+      <c r="D259" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="E259" s="2" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5" s="2" customFormat="1">
+      <c r="A260" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="B260" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C260" s="3">
+        <v>1</v>
+      </c>
+      <c r="D260" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="E260" s="2" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="261" spans="1:5" s="2" customFormat="1">
+      <c r="A261" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="B261" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C261" s="3">
+        <v>1</v>
+      </c>
+      <c r="D261" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="E261" s="2" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="262" spans="1:5" s="2" customFormat="1">
+      <c r="A262" s="2" t="s">
+        <v>661</v>
+      </c>
+      <c r="B262" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C262" s="3">
+        <v>1</v>
+      </c>
+      <c r="D262" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="E262" s="2" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="263" spans="1:5" s="2" customFormat="1">
+      <c r="A263" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="B263" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C263" s="3">
+        <v>1</v>
+      </c>
+      <c r="D263" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="E263" s="2" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="264" spans="1:5" s="2" customFormat="1">
+      <c r="A264" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="B264" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C264" s="3">
+        <v>1</v>
+      </c>
+      <c r="D264" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="E264" s="2" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="265" spans="1:5" s="2" customFormat="1">
+      <c r="A265" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="B265" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C265" s="3">
+        <v>5</v>
+      </c>
+      <c r="D265" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="E265" s="2" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="266" spans="1:5" s="2" customFormat="1">
+      <c r="A266" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="B266" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C266" s="3">
+        <v>2</v>
+      </c>
+      <c r="D266" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="E266" s="2" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="267" spans="1:5" s="2" customFormat="1">
+      <c r="A267" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="B267" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C267" s="3">
+        <v>1</v>
+      </c>
+      <c r="D267" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="E267" s="2" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="268" spans="1:5" s="2" customFormat="1">
+      <c r="A268" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="B268" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C268" s="3">
+        <v>1</v>
+      </c>
+      <c r="D268" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E268" s="2" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="269" spans="1:5" s="2" customFormat="1">
+      <c r="A269" s="2" t="s">
+        <v>663</v>
+      </c>
+      <c r="B269" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C269" s="3">
+        <v>1</v>
+      </c>
+      <c r="D269" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="E269" s="2" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="270" spans="1:5" s="2" customFormat="1">
+      <c r="A270" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="B270" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C270" s="3">
+        <v>1</v>
+      </c>
+      <c r="D270" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="E270" s="2" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="271" spans="1:5" s="2" customFormat="1">
+      <c r="A271" s="2" t="s">
+        <v>664</v>
+      </c>
+      <c r="B271" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C271" s="3">
+        <v>1</v>
+      </c>
+      <c r="D271" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="E271" s="2" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="272" spans="1:5" s="2" customFormat="1">
+      <c r="A272" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="B272" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C272" s="3">
+        <v>2</v>
+      </c>
+      <c r="D272" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="E272" s="2" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="273" spans="1:5" s="2" customFormat="1">
+      <c r="A273" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="B273" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C273" s="3">
+        <v>1</v>
+      </c>
+      <c r="D273" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="E273" s="2" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="274" spans="1:5" s="2" customFormat="1">
+      <c r="A274" s="2" t="s">
+        <v>666</v>
+      </c>
+      <c r="B274" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C274" s="3">
+        <v>1</v>
+      </c>
+      <c r="D274" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="E274" s="2" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="275" spans="1:5" s="2" customFormat="1">
+      <c r="A275" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="B275" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C275" s="3">
+        <v>2</v>
+      </c>
+      <c r="D275" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="E275" s="2" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="276" spans="1:5" s="2" customFormat="1">
+      <c r="A276" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="B276" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C276" s="3">
+        <v>5</v>
+      </c>
+      <c r="D276" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="E276" s="2" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="277" spans="1:5" s="2" customFormat="1">
+      <c r="A277" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="B277" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C277" s="3">
+        <v>1</v>
+      </c>
+      <c r="D277" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="E277" s="2" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="278" spans="1:5" s="2" customFormat="1">
+      <c r="A278" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="B278" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C278" s="3">
+        <v>1</v>
+      </c>
+      <c r="D278" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="E278" s="2" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="279" spans="1:5" s="2" customFormat="1">
+      <c r="A279" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="B279" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C279" s="3">
+        <v>5</v>
+      </c>
+      <c r="D279" s="2" t="s">
+        <v>518</v>
+      </c>
+      <c r="E279" s="2" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="280" spans="1:5" s="2" customFormat="1">
+      <c r="A280" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="B280" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C280" s="3">
+        <v>1</v>
+      </c>
+      <c r="D280" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="E280" s="2" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="281" spans="1:5" s="2" customFormat="1">
+      <c r="A281" s="2" t="s">
+        <v>526</v>
+      </c>
+      <c r="B281" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C281" s="3">
+        <v>1</v>
+      </c>
+      <c r="D281" s="2" t="s">
+        <v>527</v>
+      </c>
+      <c r="E281" s="2" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="282" spans="1:5" s="2" customFormat="1">
+      <c r="A282" s="2" t="s">
+        <v>670</v>
+      </c>
+      <c r="B282" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C282" s="3">
+        <v>1</v>
+      </c>
+      <c r="D282" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E282" s="2" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="283" spans="1:5" s="2" customFormat="1">
+      <c r="A283" s="2" t="s">
+        <v>671</v>
+      </c>
+      <c r="B283" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C283" s="3">
+        <v>5</v>
+      </c>
+      <c r="D283" s="2" t="s">
+        <v>672</v>
+      </c>
+      <c r="E283" s="2" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="284" spans="1:5" s="2" customFormat="1">
+      <c r="A284" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="B284" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C284" s="3">
+        <v>2</v>
+      </c>
+      <c r="D284" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="E284" s="2" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="285" spans="1:5" s="2" customFormat="1">
+      <c r="A285" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="B285" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C285" s="3">
+        <v>1</v>
+      </c>
+      <c r="D285" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="E285" s="2" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="286" spans="1:5" s="2" customFormat="1">
+      <c r="A286" s="2" t="s">
+        <v>676</v>
+      </c>
+      <c r="B286" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C286" s="3">
+        <v>4</v>
+      </c>
+      <c r="D286" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="E286" s="2" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="287" spans="1:5" s="2" customFormat="1">
+      <c r="A287" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="B287" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C287" s="3">
+        <v>1</v>
+      </c>
+      <c r="D287" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="E287" s="2" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="288" spans="1:5" s="2" customFormat="1">
+      <c r="A288" s="2" t="s">
+        <v>680</v>
+      </c>
+      <c r="B288" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C288" s="3">
+        <v>5</v>
+      </c>
+      <c r="D288" s="2" t="s">
+        <v>681</v>
+      </c>
+      <c r="E288" s="2" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="289" spans="1:5" s="2" customFormat="1">
+      <c r="A289" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B289" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C289" s="3">
+        <v>5</v>
+      </c>
+      <c r="D289" s="2" t="s">
+        <v>683</v>
+      </c>
+      <c r="E289" s="2" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="290" spans="1:5" s="2" customFormat="1">
+      <c r="A290" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B290" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C290" s="3">
+        <v>4</v>
+      </c>
+      <c r="D290" s="2" t="s">
+        <v>685</v>
+      </c>
+      <c r="E290" s="2" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="291" spans="1:5" s="2" customFormat="1">
+      <c r="A291" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B291" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C291" s="3">
+        <v>1</v>
+      </c>
+      <c r="D291" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="E291" s="2" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="292" spans="1:5" s="2" customFormat="1">
+      <c r="A292" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="B292" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C292" s="3">
+        <v>2</v>
+      </c>
+      <c r="D292" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="E292" s="2" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="293" spans="1:5" s="2" customFormat="1">
+      <c r="A293" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="B293" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C293" s="3">
+        <v>4</v>
+      </c>
+      <c r="D293" s="2" t="s">
+        <v>554</v>
+      </c>
+      <c r="E293" s="2" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="294" spans="1:5" s="2" customFormat="1">
+      <c r="A294" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="B294" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C294" s="3">
+        <v>2</v>
+      </c>
+      <c r="D294" s="2" t="s">
+        <v>557</v>
+      </c>
+      <c r="E294" s="2" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="295" spans="1:5" s="2" customFormat="1">
+      <c r="A295" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="B295" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C295" s="3">
+        <v>5</v>
+      </c>
+      <c r="D295" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="E295" s="2" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="296" spans="1:5" s="2" customFormat="1">
+      <c r="A296" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B296" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C296" s="3">
+        <v>3</v>
+      </c>
+      <c r="D296" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="E296" s="2" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="297" spans="1:5" s="2" customFormat="1">
+      <c r="A297" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="B297" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C297" s="3">
+        <v>4</v>
+      </c>
+      <c r="D297" s="2" t="s">
+        <v>689</v>
+      </c>
+      <c r="E297" s="2" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="298" spans="1:5" s="2" customFormat="1">
+      <c r="A298" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="B298" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C298" s="3">
+        <v>4</v>
+      </c>
+      <c r="D298" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="E298" s="2" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="299" spans="1:5" s="2" customFormat="1">
+      <c r="A299" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="B299" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C299" s="3">
+        <v>5</v>
+      </c>
+      <c r="D299" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="E299" s="2" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="300" spans="1:5" s="2" customFormat="1">
+      <c r="A300" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="B300" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C300" s="3">
+        <v>3</v>
+      </c>
+      <c r="D300" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="E300" s="2" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="301" spans="1:5" s="2" customFormat="1">
+      <c r="A301" s="2" t="s">
+        <v>691</v>
+      </c>
+      <c r="B301" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C301" s="3">
+        <v>5</v>
+      </c>
+      <c r="D301" s="2" t="s">
+        <v>692</v>
+      </c>
+      <c r="E301" s="2" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="302" spans="1:5" s="2" customFormat="1">
+      <c r="A302" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="B302" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C302" s="3">
+        <v>1</v>
+      </c>
+      <c r="D302" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="E302" s="2" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="303" spans="1:5" s="2" customFormat="1">
+      <c r="A303" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="B303" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C303" s="3">
+        <v>1</v>
+      </c>
+      <c r="D303" s="2" t="s">
+        <v>581</v>
+      </c>
+      <c r="E303" s="2" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="304" spans="1:5" s="2" customFormat="1">
+      <c r="A304" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="B304" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C304" s="3">
+        <v>1</v>
+      </c>
+      <c r="D304" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="E304" s="2" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="305" spans="1:5" s="2" customFormat="1">
+      <c r="A305" s="2" t="s">
+        <v>695</v>
+      </c>
+      <c r="B305" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C305" s="3">
+        <v>1</v>
+      </c>
+      <c r="D305" s="2" t="s">
+        <v>587</v>
+      </c>
+      <c r="E305" s="2" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="306" spans="1:5" s="2" customFormat="1">
+      <c r="A306" s="2" t="s">
+        <v>589</v>
+      </c>
+      <c r="B306" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C306" s="3">
+        <v>1</v>
+      </c>
+      <c r="D306" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="E306" s="2" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="307" spans="1:5" s="2" customFormat="1">
+      <c r="A307" s="2" t="s">
+        <v>696</v>
+      </c>
+      <c r="B307" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C307" s="3">
+        <v>1</v>
+      </c>
+      <c r="D307" s="2" t="s">
+        <v>697</v>
+      </c>
+      <c r="E307" s="2" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="308" spans="1:5" s="2" customFormat="1">
+      <c r="A308" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="B308" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C308" s="3">
+        <v>1</v>
+      </c>
+      <c r="D308" s="2" t="s">
+        <v>593</v>
+      </c>
+      <c r="E308" s="2" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="309" spans="1:5" s="2" customFormat="1">
+      <c r="A309" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B309" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C309" s="3">
+        <v>1</v>
+      </c>
+      <c r="D309" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="E309" s="2" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="310" spans="1:5" s="2" customFormat="1">
+      <c r="A310" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="B310" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C310" s="3">
+        <v>3</v>
+      </c>
+      <c r="D310" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="E310" s="2" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="311" spans="1:5" s="2" customFormat="1">
+      <c r="A311" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="B311" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C311" s="3">
+        <v>1</v>
+      </c>
+      <c r="D311" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="E311" s="2" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="312" spans="1:5" s="2" customFormat="1">
+      <c r="A312" s="2" t="s">
+        <v>700</v>
+      </c>
+      <c r="B312" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C312" s="3">
+        <v>1</v>
+      </c>
+      <c r="D312" s="2" t="s">
+        <v>701</v>
+      </c>
+      <c r="E312" s="2" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="313" spans="1:5" s="2" customFormat="1">
+      <c r="A313" s="2" t="s">
+        <v>703</v>
+      </c>
+      <c r="B313" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C313" s="3">
+        <v>2</v>
+      </c>
+      <c r="D313" s="2" t="s">
+        <v>604</v>
+      </c>
+      <c r="E313" s="2" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="314" spans="1:5" s="2" customFormat="1">
+      <c r="A314" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B314" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C314" s="3">
+        <v>1</v>
+      </c>
+      <c r="D314" s="2" t="s">
+        <v>606</v>
+      </c>
+      <c r="E314" s="2" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="315" spans="1:5" s="2" customFormat="1">
+      <c r="A315" s="2" t="s">
+        <v>704</v>
+      </c>
+      <c r="B315" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C315" s="3">
+        <v>5</v>
+      </c>
+      <c r="D315" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="E315" s="2" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="316" spans="1:5" s="2" customFormat="1">
+      <c r="A316" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="B316" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C316" s="3">
+        <v>4</v>
+      </c>
+      <c r="D316" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="E316" s="2" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="317" spans="1:5" s="2" customFormat="1">
+      <c r="A317" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B317" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C317" s="3">
+        <v>3</v>
+      </c>
+      <c r="D317" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="E317" s="2" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="318" spans="1:5" s="2" customFormat="1">
+      <c r="A318" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="B318" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C318" s="3">
+        <v>1</v>
+      </c>
+      <c r="D318" s="2" t="s">
+        <v>612</v>
+      </c>
+      <c r="E318" s="2" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="319" spans="1:5" s="2" customFormat="1">
+      <c r="A319" s="2" t="s">
+        <v>614</v>
+      </c>
+      <c r="B319" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C319" s="3">
+        <v>5</v>
+      </c>
+      <c r="D319" s="2" t="s">
+        <v>615</v>
+      </c>
+      <c r="E319" s="2" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="320" spans="1:5" s="2" customFormat="1">
+      <c r="A320" s="2" t="s">
+        <v>617</v>
+      </c>
+      <c r="B320" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C320" s="3">
+        <v>1</v>
+      </c>
+      <c r="D320" s="2" t="s">
+        <v>618</v>
+      </c>
+      <c r="E320" s="2" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="321" spans="1:5" s="2" customFormat="1">
+      <c r="A321" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="B321" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C321" s="3">
+        <v>1</v>
+      </c>
+      <c r="D321" s="2" t="s">
+        <v>621</v>
+      </c>
+      <c r="E321" s="2" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="322" spans="1:5" s="2" customFormat="1">
+      <c r="A322" s="2" t="s">
+        <v>629</v>
+      </c>
+      <c r="B322" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C322" s="3">
+        <v>1</v>
+      </c>
+      <c r="D322" s="2" t="s">
+        <v>630</v>
+      </c>
+      <c r="E322" s="2" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="323" spans="1:5" s="2" customFormat="1">
+      <c r="A323" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B323" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C323" s="3">
+        <v>1</v>
+      </c>
+      <c r="D323" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="E323" s="2" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="324" spans="1:5" s="2" customFormat="1">
+      <c r="A324" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="B324" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C324" s="3">
+        <v>1</v>
+      </c>
+      <c r="D324" s="2" t="s">
+        <v>635</v>
+      </c>
+      <c r="E324" s="2" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="325" spans="1:5" s="2" customFormat="1">
+      <c r="A325" s="2" t="s">
+        <v>637</v>
+      </c>
+      <c r="B325" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C325" s="3">
+        <v>1</v>
+      </c>
+      <c r="D325" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="E325" s="2" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="326" spans="1:5" s="2" customFormat="1">
+      <c r="A326" s="2" t="s">
+        <v>637</v>
+      </c>
+      <c r="B326" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C326" s="3">
+        <v>1</v>
+      </c>
+      <c r="D326" s="2" t="s">
+        <v>638</v>
+      </c>
+      <c r="E326" s="2" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="327" spans="1:5" s="2" customFormat="1">
+      <c r="A327" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B327" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C327" s="3">
+        <v>1</v>
+      </c>
+      <c r="D327" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="E327" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="328" spans="1:5" s="2" customFormat="1">
+      <c r="A328" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="B328" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C328" s="3">
+        <v>1</v>
+      </c>
+      <c r="D328" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="E328" s="2" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="329" spans="1:5" s="2" customFormat="1">
+      <c r="A329" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B329" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C329" s="3">
+        <v>2</v>
+      </c>
+      <c r="D329" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="E329" s="2" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="330" spans="1:5" s="2" customFormat="1">
+      <c r="A330" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="B330" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C330" s="3">
+        <v>1</v>
+      </c>
+      <c r="D330" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="E330" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="331" spans="1:5" s="2" customFormat="1">
+      <c r="A331" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="B331" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C331" s="3">
+        <v>1</v>
+      </c>
+      <c r="D331" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="E331" s="2" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="332" spans="1:5" s="2" customFormat="1">
+      <c r="A332" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="B332" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C332" s="3">
+        <v>2</v>
+      </c>
+      <c r="D332" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="E332" s="2" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="333" spans="1:5" s="2" customFormat="1">
+      <c r="A333" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="B136" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="C136" s="3">
-        <v>1</v>
-      </c>
-      <c r="D136" s="2" t="s">
+      <c r="B333" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C333" s="3">
+        <v>1</v>
+      </c>
+      <c r="D333" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="E136" s="2" t="s">
+      <c r="E333" s="2" t="s">
         <v>357</v>
       </c>
     </row>

</xml_diff>